<commit_message>
Updated BOM with to-buy details
</commit_message>
<xml_diff>
--- a/hybohat-bom.xlsx
+++ b/hybohat-bom.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rclott/root/files/projs/hybo/eda/public-hybohat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ED7971-F833-214F-B45A-97FA710BB574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC96E3F-4CF6-204D-B193-EA414625FCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59740" yWindow="5960" windowWidth="32260" windowHeight="18400" xr2:uid="{FED97CF3-E78D-5548-AD60-DA55E01ED936}"/>
+    <workbookView xWindow="51340" yWindow="4720" windowWidth="36180" windowHeight="18400" xr2:uid="{FED97CF3-E78D-5548-AD60-DA55E01ED936}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
+    <sheet name="BOM-COLORS" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="hybohat" localSheetId="0">BOM!$C$1:$U$38</definedName>
+    <definedName name="hybohat" localSheetId="0">BOM!$C$1:$S$34</definedName>
+    <definedName name="hybohat" localSheetId="1">'BOM-COLORS'!$C$1:$U$38</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +40,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{D6D63D8D-DD32-AE4C-AB18-AA43AB6E95A9}" name="hybohat" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+  <connection id="1" xr16:uid="{6DED7D30-30E6-8D4C-B5B3-623808C19CE5}" name="hybohat" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
     <textPr sourceFile="/files/projs/hybo/eda/hybohat/hybohat.csv" tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -54,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="191">
   <si>
     <t>Ref</t>
   </si>
@@ -599,6 +602,42 @@
   </si>
   <si>
     <t>RD:F2</t>
+  </si>
+  <si>
+    <t>Optional Color details below…</t>
+  </si>
+  <si>
+    <t>LK1-LK17</t>
+  </si>
+  <si>
+    <t>Must cut from 1x20 socket, this is common for ESP32 because a 1x19 is very rare</t>
+  </si>
+  <si>
+    <t>PRPC040SAAN-RC</t>
+  </si>
+  <si>
+    <t>J2-J5</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>Snap required lengths from this single 1x40 Male header</t>
+  </si>
+  <si>
+    <t>PRPC040DAAN-RC</t>
+  </si>
+  <si>
+    <t>Snap required lengths from these 2x40 Male headers</t>
+  </si>
+  <si>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>Development Module(s),  Customer Provided</t>
+  </si>
+  <si>
+    <t>ASSY</t>
   </si>
 </sst>
 </file>
@@ -608,7 +647,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -639,8 +678,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +706,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -987,7 +1052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1152,30 +1217,119 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1196,6 +1350,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hybohat" connectionId="1" xr16:uid="{E8D26DD6-51D7-EA4C-A942-7276937BBC08}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hybohat" connectionId="1" xr16:uid="{DFA7BC69-B964-C64B-B0A0-D1F18BB0752E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1495,10 +1653,2367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CBE8B4-C17B-C941-A802-EB49C9615736}">
-  <dimension ref="B1:Y76"/>
+  <dimension ref="B1:W90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="6.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
+    <col min="17" max="17" width="4" style="2" customWidth="1"/>
+    <col min="18" max="18" width="4.6640625" style="21" customWidth="1"/>
+    <col min="19" max="19" width="72.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="81"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="O1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="20"/>
+    </row>
+    <row r="2" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="83"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="O2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="20"/>
+    </row>
+    <row r="3" spans="2:23" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="78">
+        <v>44146</v>
+      </c>
+      <c r="C3" s="79"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="O3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="20"/>
+    </row>
+    <row r="4" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="O4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="20"/>
+    </row>
+    <row r="5" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:23" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1</v>
+      </c>
+      <c r="E7" s="30">
+        <v>1</v>
+      </c>
+      <c r="F7" s="30">
+        <v>1</v>
+      </c>
+      <c r="G7" s="30">
+        <v>1</v>
+      </c>
+      <c r="H7" s="30">
+        <v>1</v>
+      </c>
+      <c r="I7" s="30">
+        <v>1</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="31">
+        <v>127290</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="30"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B8" s="116">
+        <v>2</v>
+      </c>
+      <c r="C8" s="117" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118">
+        <v>1</v>
+      </c>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B9" s="116">
+        <v>3</v>
+      </c>
+      <c r="C9" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118">
+        <v>1</v>
+      </c>
+      <c r="G9" s="116"/>
+      <c r="H9" s="116"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B10" s="116">
+        <v>4</v>
+      </c>
+      <c r="C10" s="117" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118">
+        <v>1</v>
+      </c>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B11" s="116">
+        <v>5</v>
+      </c>
+      <c r="C11" s="117" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118">
+        <v>1</v>
+      </c>
+      <c r="I11" s="116"/>
+      <c r="J11" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B12" s="116">
+        <v>6</v>
+      </c>
+      <c r="C12" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118">
+        <v>1</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B13" s="7">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="9">
+        <v>387007502</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B14" s="7">
+        <v>8</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="9">
+        <v>532610871</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="W14" s="5"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B15" s="115">
+        <v>9</v>
+      </c>
+      <c r="C15" s="107" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="115">
+        <v>1</v>
+      </c>
+      <c r="E15" s="115">
+        <v>1</v>
+      </c>
+      <c r="F15" s="115">
+        <v>1</v>
+      </c>
+      <c r="G15" s="115">
+        <v>1</v>
+      </c>
+      <c r="H15" s="115">
+        <v>1</v>
+      </c>
+      <c r="I15" s="115">
+        <v>1</v>
+      </c>
+      <c r="J15" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="107"/>
+      <c r="L15" s="108"/>
+      <c r="M15" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" s="106" t="s">
+        <v>137</v>
+      </c>
+      <c r="P15" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="106" t="str">
+        <f t="shared" ref="Q15:Q37" si="0">MID($P15,1,2)</f>
+        <v>M1</v>
+      </c>
+      <c r="R15" s="109">
+        <f>VALUE(RIGHT($P15,2))*$D15</f>
+        <v>3</v>
+      </c>
+      <c r="S15" s="108" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B16" s="115">
+        <v>10</v>
+      </c>
+      <c r="C16" s="107" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="115">
+        <v>1</v>
+      </c>
+      <c r="E16" s="115">
+        <v>1</v>
+      </c>
+      <c r="F16" s="115">
+        <v>1</v>
+      </c>
+      <c r="G16" s="115">
+        <v>1</v>
+      </c>
+      <c r="H16" s="115">
+        <v>1</v>
+      </c>
+      <c r="I16" s="115">
+        <v>1</v>
+      </c>
+      <c r="J16" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="107"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="106" t="s">
+        <v>138</v>
+      </c>
+      <c r="P16" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q16" s="106" t="str">
+        <f t="shared" si="0"/>
+        <v>M1</v>
+      </c>
+      <c r="R16" s="109">
+        <f>VALUE(RIGHT($P16,2))*$D16</f>
+        <v>3</v>
+      </c>
+      <c r="S16" s="108" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="115">
+        <v>11</v>
+      </c>
+      <c r="C17" s="107" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="115">
+        <v>1</v>
+      </c>
+      <c r="E17" s="115">
+        <v>1</v>
+      </c>
+      <c r="F17" s="115">
+        <v>1</v>
+      </c>
+      <c r="G17" s="115">
+        <v>1</v>
+      </c>
+      <c r="H17" s="115">
+        <v>1</v>
+      </c>
+      <c r="I17" s="115">
+        <v>1</v>
+      </c>
+      <c r="J17" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" s="107"/>
+      <c r="L17" s="108"/>
+      <c r="M17" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17" s="106" t="s">
+        <v>139</v>
+      </c>
+      <c r="P17" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q17" s="106" t="str">
+        <f t="shared" si="0"/>
+        <v>M1</v>
+      </c>
+      <c r="R17" s="109">
+        <f>VALUE(RIGHT($P17,2))*$D17</f>
+        <v>3</v>
+      </c>
+      <c r="S17" s="108" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="115">
+        <v>12</v>
+      </c>
+      <c r="C18" s="107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="115">
+        <v>1</v>
+      </c>
+      <c r="E18" s="115">
+        <v>1</v>
+      </c>
+      <c r="F18" s="115">
+        <v>1</v>
+      </c>
+      <c r="G18" s="115">
+        <v>1</v>
+      </c>
+      <c r="H18" s="115">
+        <v>1</v>
+      </c>
+      <c r="I18" s="115">
+        <v>1</v>
+      </c>
+      <c r="J18" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="107"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="106" t="s">
+        <v>140</v>
+      </c>
+      <c r="P18" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q18" s="106" t="str">
+        <f t="shared" si="0"/>
+        <v>M1</v>
+      </c>
+      <c r="R18" s="109">
+        <f>VALUE(RIGHT($P18,2))*$D18</f>
+        <v>7</v>
+      </c>
+      <c r="S18" s="108" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B19" s="7">
+        <v>13</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R19" s="24">
+        <f>VALUE(RIGHT($P19,2))*$D19</f>
+        <v>10</v>
+      </c>
+      <c r="S19" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B20" s="7">
+        <v>14</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q20" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R20" s="24">
+        <f>VALUE(RIGHT($P20,2))*$D20</f>
+        <v>8</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="7">
+        <v>15</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="27">
+        <v>17</v>
+      </c>
+      <c r="E21" s="27">
+        <v>17</v>
+      </c>
+      <c r="F21" s="27">
+        <v>17</v>
+      </c>
+      <c r="G21" s="27">
+        <v>17</v>
+      </c>
+      <c r="H21" s="27">
+        <v>17</v>
+      </c>
+      <c r="I21" s="27">
+        <v>17</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="P21" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="74" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B22" s="7">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7">
+        <v>1</v>
+      </c>
+      <c r="I22" s="7">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" s="9">
+        <v>127581</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="7" t="str">
+        <f>MID($P22,1,2)</f>
+        <v/>
+      </c>
+      <c r="R22" s="24"/>
+      <c r="S22" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="114">
+        <v>21</v>
+      </c>
+      <c r="C23" s="100" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="114">
+        <v>2</v>
+      </c>
+      <c r="E23" s="114">
+        <v>2</v>
+      </c>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="L23" s="101" t="s">
+        <v>129</v>
+      </c>
+      <c r="M23" s="100" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="P23" s="102" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q23" s="99" t="str">
+        <f t="shared" si="0"/>
+        <v>F1</v>
+      </c>
+      <c r="R23" s="103">
+        <f>VALUE(RIGHT($P23,2))*$D23</f>
+        <v>38</v>
+      </c>
+      <c r="S23" s="101" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B24" s="110">
+        <v>22</v>
+      </c>
+      <c r="C24" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="110">
+        <v>1</v>
+      </c>
+      <c r="E24" s="110">
+        <v>1</v>
+      </c>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K24" s="91"/>
+      <c r="L24" s="92"/>
+      <c r="M24" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="O24" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="P24" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q24" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R24" s="93">
+        <f>VALUE(RIGHT($P24,2))*$D24</f>
+        <v>4</v>
+      </c>
+      <c r="S24" s="92" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B25" s="7">
+        <v>23</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q25" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>F2</v>
+      </c>
+      <c r="R25" s="24">
+        <f>VALUE(RIGHT($P25,2))*$D25</f>
+        <v>20</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="25">
+        <v>24</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="25">
+        <v>2</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25">
+        <v>2</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L26" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="M26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="N26" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="P26" s="104" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q26" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>F1</v>
+      </c>
+      <c r="R26" s="105">
+        <f>VALUE(RIGHT($P26,2))*$D26</f>
+        <v>30</v>
+      </c>
+      <c r="S26" s="74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="7">
+        <v>25</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7">
+        <v>2</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>F2</v>
+      </c>
+      <c r="R27" s="24">
+        <f>VALUE(RIGHT($P27,2))*$D27</f>
+        <v>50</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B28" s="110">
+        <v>26</v>
+      </c>
+      <c r="C28" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="110">
+        <v>1</v>
+      </c>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110">
+        <v>1</v>
+      </c>
+      <c r="I28" s="110"/>
+      <c r="J28" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" s="91"/>
+      <c r="L28" s="92"/>
+      <c r="M28" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="P28" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q28" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R28" s="93">
+        <f>VALUE(RIGHT($P28,2))*$D28</f>
+        <v>4</v>
+      </c>
+      <c r="S28" s="92" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="110">
+        <v>27</v>
+      </c>
+      <c r="C29" s="91" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="110">
+        <v>1</v>
+      </c>
+      <c r="E29" s="110"/>
+      <c r="F29" s="110"/>
+      <c r="G29" s="110"/>
+      <c r="H29" s="110">
+        <v>1</v>
+      </c>
+      <c r="I29" s="110"/>
+      <c r="J29" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" s="91"/>
+      <c r="L29" s="92"/>
+      <c r="M29" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="P29" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q29" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R29" s="93">
+        <f>VALUE(RIGHT($P29,2))*$D29</f>
+        <v>8</v>
+      </c>
+      <c r="S29" s="92" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B30" s="110">
+        <v>28</v>
+      </c>
+      <c r="C30" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="110">
+        <v>1</v>
+      </c>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110">
+        <v>1</v>
+      </c>
+      <c r="I30" s="110"/>
+      <c r="J30" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K30" s="91"/>
+      <c r="L30" s="92"/>
+      <c r="M30" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="P30" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q30" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R30" s="93">
+        <f>VALUE(RIGHT($P30,2))*$D30</f>
+        <v>8</v>
+      </c>
+      <c r="S30" s="92" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B31" s="110">
+        <v>29</v>
+      </c>
+      <c r="C31" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="110">
+        <v>1</v>
+      </c>
+      <c r="E31" s="110"/>
+      <c r="F31" s="110"/>
+      <c r="G31" s="110"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="110">
+        <v>1</v>
+      </c>
+      <c r="J31" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K31" s="91"/>
+      <c r="L31" s="92"/>
+      <c r="M31" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="O31" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P31" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q31" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R31" s="93">
+        <f>VALUE(RIGHT($P31,2))*$D31</f>
+        <v>10</v>
+      </c>
+      <c r="S31" s="92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B32" s="110">
+        <v>30</v>
+      </c>
+      <c r="C32" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="110">
+        <v>1</v>
+      </c>
+      <c r="E32" s="110"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110">
+        <v>1</v>
+      </c>
+      <c r="J32" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K32" s="91"/>
+      <c r="L32" s="92"/>
+      <c r="M32" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="N32" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="O32" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P32" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q32" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R32" s="93">
+        <f>VALUE(RIGHT($P32,2))*$D32</f>
+        <v>8</v>
+      </c>
+      <c r="S32" s="92" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B33" s="110">
+        <v>31</v>
+      </c>
+      <c r="C33" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="110">
+        <v>1</v>
+      </c>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="110"/>
+      <c r="I33" s="110">
+        <v>1</v>
+      </c>
+      <c r="J33" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K33" s="91"/>
+      <c r="L33" s="92"/>
+      <c r="M33" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="N33" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="O33" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P33" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q33" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R33" s="93">
+        <f>VALUE(RIGHT($P33,2))*$D33</f>
+        <v>15</v>
+      </c>
+      <c r="S33" s="92" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B34" s="110">
+        <v>32</v>
+      </c>
+      <c r="C34" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="110">
+        <v>1</v>
+      </c>
+      <c r="E34" s="110"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="110"/>
+      <c r="H34" s="110"/>
+      <c r="I34" s="110">
+        <v>1</v>
+      </c>
+      <c r="J34" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K34" s="91"/>
+      <c r="L34" s="92"/>
+      <c r="M34" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="O34" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P34" s="95" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q34" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R34" s="93">
+        <f>VALUE(RIGHT($P34,2))*$D34</f>
+        <v>17</v>
+      </c>
+      <c r="S34" s="92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B35" s="110">
+        <v>33</v>
+      </c>
+      <c r="C35" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="110">
+        <v>1</v>
+      </c>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="110"/>
+      <c r="I35" s="110">
+        <v>1</v>
+      </c>
+      <c r="J35" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K35" s="91"/>
+      <c r="L35" s="92"/>
+      <c r="M35" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="N35" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="O35" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P35" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q35" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R35" s="93">
+        <f>VALUE(RIGHT($P35,2))*$D35</f>
+        <v>4</v>
+      </c>
+      <c r="S35" s="92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B36" s="110">
+        <v>34</v>
+      </c>
+      <c r="C36" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="110">
+        <v>1</v>
+      </c>
+      <c r="E36" s="110"/>
+      <c r="F36" s="110"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="110"/>
+      <c r="I36" s="110">
+        <v>1</v>
+      </c>
+      <c r="J36" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K36" s="91"/>
+      <c r="L36" s="92"/>
+      <c r="M36" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="O36" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P36" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q36" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R36" s="93">
+        <f>VALUE(RIGHT($P36,2))*$D36</f>
+        <v>10</v>
+      </c>
+      <c r="S36" s="92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B37" s="110">
+        <v>35</v>
+      </c>
+      <c r="C37" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="110">
+        <v>1</v>
+      </c>
+      <c r="E37" s="110"/>
+      <c r="F37" s="110"/>
+      <c r="G37" s="110"/>
+      <c r="H37" s="110"/>
+      <c r="I37" s="110">
+        <v>1</v>
+      </c>
+      <c r="J37" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K37" s="91"/>
+      <c r="L37" s="92"/>
+      <c r="M37" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="N37" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="O37" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="P37" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q37" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>M2</v>
+      </c>
+      <c r="R37" s="93">
+        <f>VALUE(RIGHT($P37,2))*$D37</f>
+        <v>12</v>
+      </c>
+      <c r="S37" s="92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B40" s="15">
+        <v>90</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="15">
+        <v>0</v>
+      </c>
+      <c r="E40" s="15">
+        <v>0</v>
+      </c>
+      <c r="F40" s="15">
+        <v>0</v>
+      </c>
+      <c r="G40" s="15">
+        <v>0</v>
+      </c>
+      <c r="H40" s="15">
+        <v>0</v>
+      </c>
+      <c r="I40" s="15">
+        <v>0</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K40" s="16"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B41" s="111">
+        <v>91</v>
+      </c>
+      <c r="C41" s="100" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="99">
+        <v>2</v>
+      </c>
+      <c r="E41" s="99">
+        <v>2</v>
+      </c>
+      <c r="F41" s="99">
+        <v>2</v>
+      </c>
+      <c r="G41" s="99">
+        <v>2</v>
+      </c>
+      <c r="H41" s="99">
+        <v>2</v>
+      </c>
+      <c r="I41" s="99">
+        <v>2</v>
+      </c>
+      <c r="J41" s="99" t="s">
+        <v>73</v>
+      </c>
+      <c r="K41" s="100" t="s">
+        <v>125</v>
+      </c>
+      <c r="L41" s="101" t="s">
+        <v>129</v>
+      </c>
+      <c r="M41" s="100"/>
+      <c r="N41" s="100"/>
+      <c r="O41" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="P41" s="102" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q41" s="99"/>
+      <c r="R41" s="103"/>
+      <c r="S41" s="101" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B42" s="113">
+        <v>92</v>
+      </c>
+      <c r="C42" s="107" t="s">
+        <v>183</v>
+      </c>
+      <c r="D42" s="106">
+        <v>1</v>
+      </c>
+      <c r="E42" s="106">
+        <v>1</v>
+      </c>
+      <c r="F42" s="106">
+        <v>1</v>
+      </c>
+      <c r="G42" s="106">
+        <v>1</v>
+      </c>
+      <c r="H42" s="106">
+        <v>1</v>
+      </c>
+      <c r="I42" s="106">
+        <v>1</v>
+      </c>
+      <c r="J42" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="K42" s="107" t="s">
+        <v>125</v>
+      </c>
+      <c r="L42" s="108" t="s">
+        <v>182</v>
+      </c>
+      <c r="M42" s="107"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="106" t="s">
+        <v>184</v>
+      </c>
+      <c r="P42" s="106" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q42" s="106"/>
+      <c r="R42" s="109"/>
+      <c r="S42" s="107" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B43" s="112">
+        <v>93</v>
+      </c>
+      <c r="C43" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="88">
+        <v>4</v>
+      </c>
+      <c r="E43" s="88">
+        <v>4</v>
+      </c>
+      <c r="F43" s="88">
+        <v>4</v>
+      </c>
+      <c r="G43" s="88">
+        <v>4</v>
+      </c>
+      <c r="H43" s="88">
+        <v>4</v>
+      </c>
+      <c r="I43" s="88">
+        <v>4</v>
+      </c>
+      <c r="J43" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="K43" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="L43" s="92" t="s">
+        <v>186</v>
+      </c>
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
+      <c r="O43" s="88" t="s">
+        <v>184</v>
+      </c>
+      <c r="P43" s="88" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q43" s="88"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q47" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="R47" s="94">
+        <f>SUMIF($Q$7:$Q$37,$Q47,$R$7:$R$37)</f>
+        <v>16</v>
+      </c>
+      <c r="S47" s="97" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q48" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="R48" s="89">
+        <f>SUMIF($Q$7:$Q$37,$Q48,$R$7:$R$37)</f>
+        <v>118</v>
+      </c>
+      <c r="S48" s="90" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q49" s="68"/>
+      <c r="R49" s="69"/>
+      <c r="S49" s="70"/>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q50" s="68"/>
+      <c r="R50" s="69"/>
+      <c r="S50" s="70"/>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q51" s="68"/>
+      <c r="R51" s="69"/>
+      <c r="S51" s="70"/>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q52" s="68"/>
+      <c r="R52" s="69"/>
+      <c r="S52" s="70"/>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q53" s="68"/>
+      <c r="R53" s="69"/>
+      <c r="S53" s="70"/>
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="Q54" s="68"/>
+      <c r="R54" s="69"/>
+      <c r="S54" s="70"/>
+    </row>
+    <row r="55" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="84"/>
+      <c r="G55" s="84"/>
+      <c r="H55" s="84"/>
+      <c r="I55" s="84"/>
+      <c r="J55" s="84"/>
+      <c r="L55" s="85"/>
+      <c r="O55" s="84"/>
+      <c r="Q55" s="68"/>
+      <c r="R55" s="69"/>
+      <c r="S55" s="70"/>
+    </row>
+    <row r="56" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="84"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="84"/>
+      <c r="F56" s="84"/>
+      <c r="G56" s="84"/>
+      <c r="H56" s="84"/>
+      <c r="I56" s="84"/>
+      <c r="J56" s="84"/>
+      <c r="L56" s="85"/>
+      <c r="O56" s="84"/>
+      <c r="Q56" s="68"/>
+      <c r="R56" s="69"/>
+      <c r="S56" s="70"/>
+    </row>
+    <row r="57" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="84"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="84"/>
+      <c r="F57" s="84"/>
+      <c r="G57" s="84"/>
+      <c r="H57" s="84"/>
+      <c r="I57" s="84"/>
+      <c r="J57" s="84"/>
+      <c r="L57" s="85"/>
+      <c r="O57" s="84"/>
+      <c r="Q57" s="68"/>
+      <c r="R57" s="69"/>
+      <c r="S57" s="70"/>
+    </row>
+    <row r="58" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="84"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="84"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="84"/>
+      <c r="I58" s="84"/>
+      <c r="J58" s="84"/>
+      <c r="L58" s="85"/>
+      <c r="O58" s="84"/>
+      <c r="Q58" s="68"/>
+      <c r="R58" s="69"/>
+      <c r="S58" s="87"/>
+    </row>
+    <row r="59" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="84"/>
+      <c r="D59" s="84"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84"/>
+      <c r="G59" s="84"/>
+      <c r="H59" s="84"/>
+      <c r="I59" s="84"/>
+      <c r="J59" s="84"/>
+      <c r="L59" s="85"/>
+      <c r="O59" s="84"/>
+      <c r="Q59" s="68"/>
+      <c r="R59" s="69"/>
+      <c r="S59" s="87"/>
+    </row>
+    <row r="60" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="84"/>
+      <c r="D60" s="84"/>
+      <c r="E60" s="84"/>
+      <c r="F60" s="84"/>
+      <c r="G60" s="84"/>
+      <c r="H60" s="84"/>
+      <c r="I60" s="84"/>
+      <c r="J60" s="84"/>
+      <c r="L60" s="85"/>
+      <c r="O60" s="84"/>
+      <c r="Q60" s="68"/>
+      <c r="R60" s="69"/>
+      <c r="S60" s="70"/>
+    </row>
+    <row r="61" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="84"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="84"/>
+      <c r="F61" s="84"/>
+      <c r="G61" s="84"/>
+      <c r="H61" s="84"/>
+      <c r="I61" s="84"/>
+      <c r="J61" s="84"/>
+      <c r="L61" s="85"/>
+      <c r="O61" s="84"/>
+      <c r="Q61" s="68"/>
+      <c r="R61" s="69"/>
+      <c r="S61" s="70"/>
+    </row>
+    <row r="62" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="84"/>
+      <c r="D62" s="84"/>
+      <c r="E62" s="84"/>
+      <c r="F62" s="84"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="84"/>
+      <c r="I62" s="84"/>
+      <c r="J62" s="84"/>
+      <c r="L62" s="85"/>
+      <c r="O62" s="84"/>
+      <c r="Q62" s="68"/>
+      <c r="R62" s="69"/>
+      <c r="S62" s="70"/>
+    </row>
+    <row r="63" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="84"/>
+      <c r="D63" s="84"/>
+      <c r="E63" s="84"/>
+      <c r="F63" s="84"/>
+      <c r="G63" s="84"/>
+      <c r="H63" s="84"/>
+      <c r="I63" s="84"/>
+      <c r="J63" s="84"/>
+      <c r="L63" s="85"/>
+      <c r="O63" s="84"/>
+      <c r="Q63" s="68"/>
+      <c r="R63" s="69"/>
+      <c r="S63" s="70"/>
+    </row>
+    <row r="64" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="84"/>
+      <c r="D64" s="84"/>
+      <c r="E64" s="84"/>
+      <c r="F64" s="84"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="84"/>
+      <c r="I64" s="84"/>
+      <c r="J64" s="84"/>
+      <c r="L64" s="85"/>
+      <c r="O64" s="84"/>
+      <c r="Q64" s="68"/>
+      <c r="R64" s="69"/>
+      <c r="S64" s="70"/>
+    </row>
+    <row r="65" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="84"/>
+      <c r="F65" s="84"/>
+      <c r="G65" s="84"/>
+      <c r="H65" s="84"/>
+      <c r="I65" s="84"/>
+      <c r="J65" s="84"/>
+      <c r="L65" s="85"/>
+      <c r="O65" s="84"/>
+      <c r="Q65" s="68"/>
+      <c r="R65" s="69"/>
+      <c r="S65" s="70"/>
+    </row>
+    <row r="66" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="84"/>
+      <c r="D66" s="84"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="84"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="84"/>
+      <c r="I66" s="84"/>
+      <c r="J66" s="84"/>
+      <c r="L66" s="85"/>
+      <c r="O66" s="84"/>
+      <c r="Q66" s="68"/>
+      <c r="R66" s="69"/>
+      <c r="S66" s="70"/>
+    </row>
+    <row r="67" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="84"/>
+      <c r="D67" s="84"/>
+      <c r="E67" s="84"/>
+      <c r="F67" s="84"/>
+      <c r="G67" s="84"/>
+      <c r="H67" s="84"/>
+      <c r="I67" s="84"/>
+      <c r="J67" s="84"/>
+      <c r="L67" s="85"/>
+      <c r="O67" s="84"/>
+      <c r="Q67" s="68"/>
+      <c r="R67" s="69"/>
+      <c r="S67" s="70"/>
+    </row>
+    <row r="68" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="84"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="84"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="84"/>
+      <c r="I68" s="84"/>
+      <c r="J68" s="84"/>
+      <c r="L68" s="85"/>
+      <c r="O68" s="84"/>
+      <c r="Q68" s="68"/>
+      <c r="R68" s="69"/>
+      <c r="S68" s="70"/>
+    </row>
+    <row r="69" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="84"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="84"/>
+      <c r="F69" s="84"/>
+      <c r="G69" s="84"/>
+      <c r="H69" s="84"/>
+      <c r="I69" s="84"/>
+      <c r="J69" s="84"/>
+      <c r="L69" s="85"/>
+      <c r="O69" s="84"/>
+      <c r="Q69" s="68"/>
+      <c r="R69" s="69"/>
+      <c r="S69" s="70"/>
+    </row>
+    <row r="70" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="84"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="84"/>
+      <c r="G70" s="84"/>
+      <c r="H70" s="84"/>
+      <c r="I70" s="84"/>
+      <c r="J70" s="84"/>
+      <c r="L70" s="85"/>
+      <c r="O70" s="84"/>
+      <c r="Q70" s="68"/>
+      <c r="R70" s="69"/>
+      <c r="S70" s="70"/>
+    </row>
+    <row r="71" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="84"/>
+      <c r="D71" s="84"/>
+      <c r="E71" s="84"/>
+      <c r="F71" s="84"/>
+      <c r="G71" s="84"/>
+      <c r="H71" s="84"/>
+      <c r="I71" s="84"/>
+      <c r="J71" s="84"/>
+      <c r="L71" s="85"/>
+      <c r="O71" s="84"/>
+      <c r="Q71" s="68"/>
+      <c r="R71" s="69"/>
+      <c r="S71" s="70"/>
+    </row>
+    <row r="72" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="84"/>
+      <c r="D72" s="84"/>
+      <c r="E72" s="84"/>
+      <c r="F72" s="84"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="84"/>
+      <c r="I72" s="84"/>
+      <c r="J72" s="84"/>
+      <c r="L72" s="85"/>
+      <c r="O72" s="84"/>
+      <c r="Q72" s="68"/>
+      <c r="R72" s="69"/>
+      <c r="S72" s="70"/>
+    </row>
+    <row r="73" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="84"/>
+      <c r="D73" s="84"/>
+      <c r="E73" s="84"/>
+      <c r="F73" s="84"/>
+      <c r="G73" s="84"/>
+      <c r="H73" s="84"/>
+      <c r="I73" s="84"/>
+      <c r="J73" s="84"/>
+      <c r="L73" s="85"/>
+      <c r="O73" s="84"/>
+      <c r="Q73" s="68"/>
+      <c r="R73" s="69"/>
+      <c r="S73" s="70"/>
+    </row>
+    <row r="74" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="84"/>
+      <c r="D74" s="84"/>
+      <c r="E74" s="84"/>
+      <c r="F74" s="84"/>
+      <c r="G74" s="84"/>
+      <c r="H74" s="84"/>
+      <c r="I74" s="84"/>
+      <c r="J74" s="84"/>
+      <c r="L74" s="85"/>
+      <c r="O74" s="84"/>
+      <c r="Q74" s="68"/>
+      <c r="R74" s="69"/>
+      <c r="S74" s="70"/>
+    </row>
+    <row r="75" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="84"/>
+      <c r="D75" s="84"/>
+      <c r="E75" s="84"/>
+      <c r="F75" s="84"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="84"/>
+      <c r="I75" s="84"/>
+      <c r="J75" s="84"/>
+      <c r="L75" s="85"/>
+      <c r="O75" s="84"/>
+      <c r="Q75" s="68"/>
+      <c r="R75" s="69"/>
+      <c r="S75" s="70"/>
+    </row>
+    <row r="76" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="84"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="84"/>
+      <c r="F76" s="84"/>
+      <c r="G76" s="84"/>
+      <c r="H76" s="84"/>
+      <c r="I76" s="84"/>
+      <c r="J76" s="84"/>
+      <c r="L76" s="85"/>
+      <c r="O76" s="84"/>
+      <c r="Q76" s="68"/>
+      <c r="R76" s="69"/>
+      <c r="S76" s="70"/>
+    </row>
+    <row r="77" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="84"/>
+      <c r="D77" s="84"/>
+      <c r="E77" s="84"/>
+      <c r="F77" s="84"/>
+      <c r="G77" s="84"/>
+      <c r="H77" s="84"/>
+      <c r="I77" s="84"/>
+      <c r="J77" s="84"/>
+      <c r="L77" s="85"/>
+      <c r="O77" s="84"/>
+      <c r="Q77" s="68"/>
+      <c r="R77" s="69"/>
+      <c r="S77" s="70"/>
+    </row>
+    <row r="78" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="84"/>
+      <c r="D78" s="84"/>
+      <c r="E78" s="84"/>
+      <c r="F78" s="84"/>
+      <c r="G78" s="84"/>
+      <c r="H78" s="84"/>
+      <c r="I78" s="84"/>
+      <c r="J78" s="84"/>
+      <c r="L78" s="85"/>
+      <c r="O78" s="84"/>
+      <c r="Q78" s="68"/>
+      <c r="R78" s="69"/>
+      <c r="S78" s="70"/>
+    </row>
+    <row r="79" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="84"/>
+      <c r="D79" s="84"/>
+      <c r="E79" s="84"/>
+      <c r="F79" s="84"/>
+      <c r="G79" s="84"/>
+      <c r="H79" s="84"/>
+      <c r="I79" s="84"/>
+      <c r="J79" s="84"/>
+      <c r="L79" s="85"/>
+      <c r="O79" s="84"/>
+      <c r="Q79" s="68"/>
+      <c r="R79" s="69"/>
+      <c r="S79" s="70"/>
+    </row>
+    <row r="80" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="84"/>
+      <c r="D80" s="84"/>
+      <c r="E80" s="84"/>
+      <c r="F80" s="84"/>
+      <c r="G80" s="84"/>
+      <c r="H80" s="84"/>
+      <c r="I80" s="84"/>
+      <c r="J80" s="84"/>
+      <c r="L80" s="85"/>
+      <c r="O80" s="84"/>
+      <c r="Q80" s="68"/>
+      <c r="R80" s="69"/>
+      <c r="S80" s="70"/>
+    </row>
+    <row r="81" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="84"/>
+      <c r="D81" s="84"/>
+      <c r="E81" s="84"/>
+      <c r="F81" s="84"/>
+      <c r="G81" s="84"/>
+      <c r="H81" s="84"/>
+      <c r="I81" s="84"/>
+      <c r="J81" s="84"/>
+      <c r="L81" s="85"/>
+      <c r="O81" s="84"/>
+      <c r="Q81" s="68"/>
+      <c r="R81" s="69"/>
+      <c r="S81" s="70"/>
+    </row>
+    <row r="82" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="84"/>
+      <c r="D82" s="84"/>
+      <c r="E82" s="84"/>
+      <c r="F82" s="84"/>
+      <c r="G82" s="84"/>
+      <c r="H82" s="84"/>
+      <c r="I82" s="84"/>
+      <c r="J82" s="84"/>
+      <c r="L82" s="85"/>
+      <c r="O82" s="84"/>
+      <c r="Q82" s="68"/>
+      <c r="R82" s="69"/>
+      <c r="S82" s="70"/>
+    </row>
+    <row r="83" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="84"/>
+      <c r="D83" s="84"/>
+      <c r="E83" s="84"/>
+      <c r="F83" s="84"/>
+      <c r="G83" s="84"/>
+      <c r="H83" s="84"/>
+      <c r="I83" s="84"/>
+      <c r="J83" s="84"/>
+      <c r="L83" s="85"/>
+      <c r="O83" s="84"/>
+      <c r="Q83" s="68"/>
+      <c r="R83" s="69"/>
+      <c r="S83" s="70"/>
+    </row>
+    <row r="84" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="84"/>
+      <c r="D84" s="84"/>
+      <c r="E84" s="84"/>
+      <c r="F84" s="84"/>
+      <c r="G84" s="84"/>
+      <c r="H84" s="84"/>
+      <c r="I84" s="84"/>
+      <c r="J84" s="84"/>
+      <c r="L84" s="85"/>
+      <c r="O84" s="84"/>
+      <c r="Q84" s="68"/>
+      <c r="R84" s="69"/>
+      <c r="S84" s="70"/>
+    </row>
+    <row r="85" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="84"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="84"/>
+      <c r="F85" s="84"/>
+      <c r="G85" s="84"/>
+      <c r="H85" s="84"/>
+      <c r="I85" s="84"/>
+      <c r="J85" s="84"/>
+      <c r="L85" s="85"/>
+      <c r="O85" s="84"/>
+      <c r="Q85" s="68"/>
+      <c r="R85" s="69"/>
+      <c r="S85" s="70"/>
+    </row>
+    <row r="86" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="84"/>
+      <c r="D86" s="84"/>
+      <c r="E86" s="84"/>
+      <c r="F86" s="84"/>
+      <c r="G86" s="84"/>
+      <c r="H86" s="84"/>
+      <c r="I86" s="84"/>
+      <c r="J86" s="84"/>
+      <c r="L86" s="85"/>
+      <c r="O86" s="84"/>
+      <c r="Q86" s="68"/>
+      <c r="R86" s="69"/>
+      <c r="S86" s="70"/>
+    </row>
+    <row r="87" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="84"/>
+      <c r="D87" s="84"/>
+      <c r="E87" s="84"/>
+      <c r="F87" s="84"/>
+      <c r="G87" s="84"/>
+      <c r="H87" s="84"/>
+      <c r="I87" s="84"/>
+      <c r="J87" s="84"/>
+      <c r="L87" s="85"/>
+      <c r="O87" s="84"/>
+      <c r="Q87" s="68"/>
+      <c r="R87" s="69"/>
+      <c r="S87" s="70"/>
+    </row>
+    <row r="88" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="84"/>
+      <c r="D88" s="84"/>
+      <c r="E88" s="84"/>
+      <c r="F88" s="84"/>
+      <c r="G88" s="84"/>
+      <c r="H88" s="84"/>
+      <c r="I88" s="84"/>
+      <c r="J88" s="84"/>
+      <c r="L88" s="85"/>
+      <c r="O88" s="84"/>
+      <c r="Q88" s="84"/>
+      <c r="R88" s="86"/>
+    </row>
+    <row r="89" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="84"/>
+      <c r="D89" s="84"/>
+      <c r="E89" s="84"/>
+      <c r="F89" s="84"/>
+      <c r="G89" s="84"/>
+      <c r="H89" s="84"/>
+      <c r="I89" s="84"/>
+      <c r="J89" s="84"/>
+      <c r="L89" s="85"/>
+      <c r="O89" s="84"/>
+      <c r="Q89" s="84"/>
+      <c r="R89" s="86"/>
+    </row>
+    <row r="90" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="84"/>
+      <c r="D90" s="84"/>
+      <c r="E90" s="84"/>
+      <c r="F90" s="84"/>
+      <c r="G90" s="84"/>
+      <c r="H90" s="84"/>
+      <c r="I90" s="84"/>
+      <c r="J90" s="84"/>
+      <c r="L90" s="85"/>
+      <c r="O90" s="84"/>
+      <c r="Q90" s="84"/>
+      <c r="R90" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EAADE6-4264-DE47-A067-ABBE604B6FE0}">
+  <dimension ref="A1:Y83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1522,10 +4037,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="77"/>
+      <c r="C1" s="81"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1541,10 +4056,10 @@
       <c r="T1" s="20"/>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="79"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1560,10 +4075,10 @@
       <c r="T2" s="20"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="74">
+      <c r="B3" s="78">
         <v>44146</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -2016,11 +4531,11 @@
         <v>68</v>
       </c>
       <c r="R15" s="9" t="str">
-        <f>CONCATENATE(MID($P15,1,1),RIGHT($P15,1),":",MID($Q15,1,2))</f>
+        <f t="shared" ref="R15:R20" si="0">CONCATENATE(MID($P15,1,1),RIGHT($P15,1),":",MID($Q15,1,2))</f>
         <v>BE:M1</v>
       </c>
       <c r="S15" s="7" t="str">
-        <f t="shared" ref="R15:S41" si="0">MID($Q15,1,2)</f>
+        <f t="shared" ref="S15:S41" si="1">MID($Q15,1,2)</f>
         <v>M1</v>
       </c>
       <c r="T15" s="24">
@@ -2077,15 +4592,15 @@
         <v>68</v>
       </c>
       <c r="R16" s="9" t="str">
-        <f>CONCATENATE(MID($P16,1,1),RIGHT($P16,1),":",MID($Q16,1,2))</f>
+        <f t="shared" si="0"/>
         <v>GN:M1</v>
       </c>
       <c r="S16" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M1</v>
       </c>
       <c r="T16" s="24">
-        <f t="shared" ref="T16:T17" si="1">VALUE(RIGHT($Q16,2))*$D16</f>
+        <f t="shared" ref="T16:T17" si="2">VALUE(RIGHT($Q16,2))*$D16</f>
         <v>3</v>
       </c>
       <c r="U16" s="9" t="s">
@@ -2138,15 +4653,15 @@
         <v>68</v>
       </c>
       <c r="R17" s="9" t="str">
-        <f>CONCATENATE(MID($P17,1,1),RIGHT($P17,1),":",MID($Q17,1,2))</f>
+        <f t="shared" si="0"/>
         <v>BK:M1</v>
       </c>
       <c r="S17" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M1</v>
       </c>
       <c r="T17" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="U17" s="9" t="s">
@@ -2199,11 +4714,11 @@
         <v>69</v>
       </c>
       <c r="R18" s="9" t="str">
-        <f>CONCATENATE(MID($P18,1,1),RIGHT($P18,1),":",MID($Q18,1,2))</f>
+        <f t="shared" si="0"/>
         <v>YW:M1</v>
       </c>
       <c r="S18" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M1</v>
       </c>
       <c r="T18" s="24">
@@ -2260,11 +4775,11 @@
         <v>55</v>
       </c>
       <c r="R19" s="9" t="str">
-        <f>CONCATENATE(MID($P19,1,1),RIGHT($P19,1),":",MID($Q19,1,2))</f>
+        <f t="shared" si="0"/>
         <v>RD:M2</v>
       </c>
       <c r="S19" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T19" s="24">
@@ -2321,11 +4836,11 @@
         <v>59</v>
       </c>
       <c r="R20" s="9" t="str">
-        <f>CONCATENATE(MID($P20,1,1),RIGHT($P20,1),":",MID($Q20,1,2))</f>
+        <f t="shared" si="0"/>
         <v>BK:M2</v>
       </c>
       <c r="S20" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T20" s="24">
@@ -2340,7 +4855,7 @@
       <c r="B21" s="7">
         <v>15</v>
       </c>
-      <c r="C21" s="81" t="s">
+      <c r="C21" s="75" t="s">
         <v>145</v>
       </c>
       <c r="D21" s="27">
@@ -2381,7 +4896,7 @@
       <c r="Q21" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="R21" s="80"/>
+      <c r="R21" s="74"/>
       <c r="S21" s="25"/>
       <c r="T21" s="24"/>
       <c r="U21" s="37" t="s">
@@ -2392,7 +4907,7 @@
       <c r="B22" s="7">
         <v>16</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="75" t="s">
         <v>146</v>
       </c>
       <c r="D22" s="27">
@@ -2433,7 +4948,7 @@
       <c r="Q22" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="R22" s="80"/>
+      <c r="R22" s="74"/>
       <c r="S22" s="25"/>
       <c r="T22" s="24"/>
       <c r="U22" s="37" t="s">
@@ -2444,7 +4959,7 @@
       <c r="B23" s="7">
         <v>17</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="75" t="s">
         <v>148</v>
       </c>
       <c r="D23" s="27">
@@ -2485,7 +5000,7 @@
       <c r="Q23" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="R23" s="80"/>
+      <c r="R23" s="74"/>
       <c r="S23" s="25"/>
       <c r="T23" s="24"/>
       <c r="U23" s="37" t="s">
@@ -2496,7 +5011,7 @@
       <c r="B24" s="7">
         <v>18</v>
       </c>
-      <c r="C24" s="81" t="s">
+      <c r="C24" s="75" t="s">
         <v>150</v>
       </c>
       <c r="D24" s="27">
@@ -2537,7 +5052,7 @@
       <c r="Q24" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="R24" s="80"/>
+      <c r="R24" s="74"/>
       <c r="S24" s="25"/>
       <c r="T24" s="24"/>
       <c r="U24" s="37" t="s">
@@ -2548,7 +5063,7 @@
       <c r="B25" s="7">
         <v>19</v>
       </c>
-      <c r="C25" s="81" t="s">
+      <c r="C25" s="75" t="s">
         <v>152</v>
       </c>
       <c r="D25" s="27">
@@ -2589,7 +5104,7 @@
       <c r="Q25" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="R25" s="80"/>
+      <c r="R25" s="74"/>
       <c r="S25" s="25"/>
       <c r="T25" s="24"/>
       <c r="U25" s="37" t="s">
@@ -2600,7 +5115,7 @@
       <c r="B26" s="7">
         <v>20</v>
       </c>
-      <c r="C26" s="82"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="39">
         <v>1</v>
       </c>
@@ -2685,15 +5200,15 @@
         <v>61</v>
       </c>
       <c r="R27" s="9" t="str">
-        <f>CONCATENATE(MID($P27,1,1),RIGHT($P27,1),":",MID($Q27,1,2))</f>
+        <f t="shared" ref="R27:R41" si="3">CONCATENATE(MID($P27,1,1),RIGHT($P27,1),":",MID($Q27,1,2))</f>
         <v>BE:F1</v>
       </c>
       <c r="S27" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F1</v>
       </c>
       <c r="T27" s="32">
-        <f t="shared" ref="T27:T41" si="2">VALUE(RIGHT($Q27,2))*$D27</f>
+        <f t="shared" ref="T27:T41" si="4">VALUE(RIGHT($Q27,2))*$D27</f>
         <v>38</v>
       </c>
       <c r="U27" s="44" t="s">
@@ -2704,7 +5219,7 @@
       <c r="B28" s="7">
         <v>22</v>
       </c>
-      <c r="C28" s="82" t="s">
+      <c r="C28" s="76" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="39">
@@ -2738,15 +5253,15 @@
         <v>58</v>
       </c>
       <c r="R28" s="9" t="str">
-        <f>CONCATENATE(MID($P28,1,1),RIGHT($P28,1),":",MID($Q28,1,2))</f>
+        <f t="shared" si="3"/>
         <v>GN:M2</v>
       </c>
       <c r="S28" s="39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T28" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U28" s="45" t="s">
@@ -2757,7 +5272,7 @@
       <c r="B29" s="7">
         <v>23</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="77" t="s">
         <v>35</v>
       </c>
       <c r="D29" s="47">
@@ -2795,15 +5310,15 @@
         <v>62</v>
       </c>
       <c r="R29" s="9" t="str">
-        <f>CONCATENATE(MID($P29,1,1),RIGHT($P29,1),":",MID($Q29,1,2))</f>
+        <f t="shared" si="3"/>
         <v>RD:F2</v>
       </c>
       <c r="S29" s="47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F2</v>
       </c>
       <c r="T29" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="U29" s="51" t="s">
@@ -2814,7 +5329,7 @@
       <c r="B30" s="7">
         <v>24</v>
       </c>
-      <c r="C30" s="83" t="s">
+      <c r="C30" s="77" t="s">
         <v>107</v>
       </c>
       <c r="D30" s="47">
@@ -2852,15 +5367,15 @@
         <v>63</v>
       </c>
       <c r="R30" s="9" t="str">
-        <f>CONCATENATE(MID($P30,1,1),RIGHT($P30,1),":",MID($Q30,1,2))</f>
+        <f t="shared" si="3"/>
         <v>YW:F1</v>
       </c>
       <c r="S30" s="47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F1</v>
       </c>
       <c r="T30" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="U30" s="51" t="s">
@@ -2909,15 +5424,15 @@
         <v>64</v>
       </c>
       <c r="R31" s="9" t="str">
-        <f>CONCATENATE(MID($P31,1,1),RIGHT($P31,1),":",MID($Q31,1,2))</f>
+        <f t="shared" si="3"/>
         <v>BK:F2</v>
       </c>
       <c r="S31" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>F2</v>
       </c>
       <c r="T31" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="U31" s="44" t="s">
@@ -2962,15 +5477,15 @@
         <v>58</v>
       </c>
       <c r="R32" s="9" t="str">
-        <f>CONCATENATE(MID($P32,1,1),RIGHT($P32,1),":",MID($Q32,1,2))</f>
+        <f t="shared" si="3"/>
         <v>BE:M2</v>
       </c>
       <c r="S32" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T32" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U32" s="36" t="s">
@@ -3015,15 +5530,15 @@
         <v>59</v>
       </c>
       <c r="R33" s="9" t="str">
-        <f>CONCATENATE(MID($P33,1,1),RIGHT($P33,1),":",MID($Q33,1,2))</f>
+        <f t="shared" si="3"/>
         <v>GN:M2</v>
       </c>
       <c r="S33" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T33" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="U33" s="36" t="s">
@@ -3034,7 +5549,7 @@
       <c r="B34" s="7">
         <v>28</v>
       </c>
-      <c r="C34" s="82" t="s">
+      <c r="C34" s="76" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="39">
@@ -3068,15 +5583,15 @@
         <v>59</v>
       </c>
       <c r="R34" s="9" t="str">
-        <f>CONCATENATE(MID($P34,1,1),RIGHT($P34,1),":",MID($Q34,1,2))</f>
+        <f t="shared" si="3"/>
         <v>YW:M2</v>
       </c>
       <c r="S34" s="39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T34" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="U34" s="45" t="s">
@@ -3121,15 +5636,15 @@
         <v>55</v>
       </c>
       <c r="R35" s="9" t="str">
-        <f>CONCATENATE(MID($P35,1,1),RIGHT($P35,1),":",MID($Q35,1,2))</f>
+        <f t="shared" si="3"/>
         <v>WE:M2</v>
       </c>
       <c r="S35" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T35" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="U35" s="44" t="s">
@@ -3174,15 +5689,15 @@
         <v>59</v>
       </c>
       <c r="R36" s="9" t="str">
-        <f>CONCATENATE(MID($P36,1,1),RIGHT($P36,1),":",MID($Q36,1,2))</f>
+        <f t="shared" si="3"/>
         <v>WE:M2</v>
       </c>
       <c r="S36" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T36" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="U36" s="36" t="s">
@@ -3227,15 +5742,15 @@
         <v>65</v>
       </c>
       <c r="R37" s="9" t="str">
-        <f>CONCATENATE(MID($P37,1,1),RIGHT($P37,1),":",MID($Q37,1,2))</f>
+        <f t="shared" si="3"/>
         <v>WE:M2</v>
       </c>
       <c r="S37" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T37" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="U37" s="36" t="s">
@@ -3280,15 +5795,15 @@
         <v>66</v>
       </c>
       <c r="R38" s="9" t="str">
-        <f>CONCATENATE(MID($P38,1,1),RIGHT($P38,1),":",MID($Q38,1,2))</f>
+        <f t="shared" si="3"/>
         <v>WE:M2</v>
       </c>
       <c r="S38" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T38" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="U38" s="36" t="s">
@@ -3333,15 +5848,15 @@
         <v>58</v>
       </c>
       <c r="R39" s="9" t="str">
-        <f>CONCATENATE(MID($P39,1,1),RIGHT($P39,1),":",MID($Q39,1,2))</f>
+        <f t="shared" si="3"/>
         <v>BE:M2</v>
       </c>
       <c r="S39" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T39" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U39" s="36" t="s">
@@ -3386,15 +5901,15 @@
         <v>55</v>
       </c>
       <c r="R40" s="9" t="str">
-        <f>CONCATENATE(MID($P40,1,1),RIGHT($P40,1),":",MID($Q40,1,2))</f>
+        <f t="shared" si="3"/>
         <v>GN:M2</v>
       </c>
       <c r="S40" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T40" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="U40" s="36" t="s">
@@ -3405,7 +5920,7 @@
       <c r="B41" s="7">
         <v>35</v>
       </c>
-      <c r="C41" s="82" t="s">
+      <c r="C41" s="76" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="39">
@@ -3439,15 +5954,15 @@
         <v>60</v>
       </c>
       <c r="R41" s="9" t="str">
-        <f>CONCATENATE(MID($P41,1,1),RIGHT($P41,1),":",MID($Q41,1,2))</f>
+        <f t="shared" si="3"/>
         <v>YW:M2</v>
       </c>
       <c r="S41" s="39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>M2</v>
       </c>
       <c r="T41" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="U41" s="45" t="s">
@@ -3479,246 +5994,284 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
       <c r="S47" s="68"/>
       <c r="T47" s="69"/>
       <c r="U47" s="70"/>
     </row>
-    <row r="48" spans="2:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R48" s="4" t="s">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="S48" s="68"/>
+      <c r="T48" s="69"/>
+      <c r="U48" s="70"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S49" s="68"/>
+      <c r="T49" s="69"/>
+      <c r="U49" s="70"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S50" s="68"/>
+      <c r="T50" s="69"/>
+      <c r="U50" s="70"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S51" s="68"/>
+      <c r="T51" s="69"/>
+      <c r="U51" s="70"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S52" s="68"/>
+      <c r="T52" s="69"/>
+      <c r="U52" s="70"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>179</v>
+      </c>
+      <c r="S53" s="68"/>
+      <c r="T53" s="69"/>
+      <c r="U53" s="70"/>
+    </row>
+    <row r="54" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S54" s="68"/>
+      <c r="T54" s="69"/>
+      <c r="U54" s="70"/>
+    </row>
+    <row r="55" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R55" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="S48" s="68"/>
-      <c r="T48" s="58">
-        <f>SUMIF($R$7:$R$41,$R48,$T$7:$T$41)</f>
-        <v>0</v>
-      </c>
-      <c r="U48" s="70"/>
-    </row>
-    <row r="49" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R49" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="T49" s="58">
-        <f>SUMIF($R$7:$R$41,$R49,$T$7:$T$41)</f>
-        <v>50</v>
-      </c>
-      <c r="U49" s="4"/>
-    </row>
-    <row r="50" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R50" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="T50" s="58">
-        <f>SUMIF($R$7:$R$41,$R50,$T$7:$T$41)</f>
-        <v>0</v>
-      </c>
-      <c r="U50" s="4"/>
-    </row>
-    <row r="51" spans="18:21" x14ac:dyDescent="0.2">
-      <c r="R51" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="T51" s="58">
-        <f>SUMIF($R$7:$R$41,$R51,$T$7:$T$41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R53" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="S53" s="68"/>
-      <c r="T53" s="58">
-        <f>SUMIF($R$7:$R$41,$R53,$T$7:$T$41)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R54" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="T54" s="58">
-        <f>SUMIF($R$7:$R$41,$R54,$T$7:$T$41)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R55" s="4" t="s">
-        <v>161</v>
-      </c>
+      <c r="S55" s="68"/>
       <c r="T55" s="58">
         <f>SUMIF($R$7:$R$41,$R55,$T$7:$T$41)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="18:21" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="U55" s="70"/>
+    </row>
+    <row r="56" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R56" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="T56" s="58">
         <f>SUMIF($R$7:$R$41,$R56,$T$7:$T$41)</f>
+        <v>50</v>
+      </c>
+      <c r="U56" s="4"/>
+    </row>
+    <row r="57" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R57" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="T57" s="58">
+        <f>SUMIF($R$7:$R$41,$R57,$T$7:$T$41)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U57" s="4"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="R58" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="S58" s="68"/>
+        <v>158</v>
+      </c>
       <c r="T58" s="58">
         <f>SUMIF($R$7:$R$41,$R58,$T$7:$T$41)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R59" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="T59" s="58">
-        <f>SUMIF($R$7:$R$41,$R59,$T$7:$T$41)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R60" s="4" t="s">
-        <v>165</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="S60" s="68"/>
       <c r="T60" s="58">
         <f>SUMIF($R$7:$R$41,$R60,$T$7:$T$41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="18:21" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R61" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="T61" s="58">
         <f>SUMIF($R$7:$R$41,$R61,$T$7:$T$41)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R62" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="T62" s="58">
+        <f>SUMIF($R$7:$R$41,$R62,$T$7:$T$41)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="R63" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="S63" s="68"/>
+        <v>162</v>
+      </c>
       <c r="T63" s="58">
         <f>SUMIF($R$7:$R$41,$R63,$T$7:$T$41)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="18:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R64" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="T64" s="58">
-        <f>SUMIF($R$7:$R$41,$R64,$T$7:$T$41)</f>
-        <v>22</v>
-      </c>
-    </row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R65" s="4" t="s">
-        <v>170</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="S65" s="68"/>
       <c r="T65" s="58">
         <f>SUMIF($R$7:$R$41,$R65,$T$7:$T$41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="18:20" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R66" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="T66" s="58">
         <f>SUMIF($R$7:$R$41,$R66,$T$7:$T$41)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R67" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="T67" s="58">
+        <f>SUMIF($R$7:$R$41,$R67,$T$7:$T$41)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="18:20" x14ac:dyDescent="0.2">
       <c r="R68" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="S68" s="68"/>
+        <v>166</v>
+      </c>
       <c r="T68" s="58">
         <f>SUMIF($R$7:$R$41,$R68,$T$7:$T$41)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R69" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="T69" s="58">
-        <f>SUMIF($R$7:$R$41,$R69,$T$7:$T$41)</f>
-        <v>20</v>
-      </c>
-    </row>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R70" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="S70" s="68"/>
       <c r="T70" s="58">
         <f>SUMIF($R$7:$R$41,$R70,$T$7:$T$41)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="18:20" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R71" s="4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="T71" s="58">
         <f>SUMIF($R$7:$R$41,$R71,$T$7:$T$41)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R72" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="T72" s="58">
+        <f>SUMIF($R$7:$R$41,$R72,$T$7:$T$41)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="18:20" x14ac:dyDescent="0.2">
       <c r="R73" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="S73" s="68"/>
+        <v>169</v>
+      </c>
       <c r="T73" s="58">
         <f>SUMIF($R$7:$R$41,$R73,$T$7:$T$41)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R74" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="T74" s="58">
-        <f>SUMIF($R$7:$R$41,$R74,$T$7:$T$41)</f>
-        <v>10</v>
-      </c>
-    </row>
+    <row r="74" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R75" s="4" t="s">
-        <v>177</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="S75" s="68"/>
       <c r="T75" s="58">
         <f>SUMIF($R$7:$R$41,$R75,$T$7:$T$41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="18:20" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="R76" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="T76" s="58">
         <f>SUMIF($R$7:$R$41,$R76,$T$7:$T$41)</f>
         <v>20</v>
       </c>
     </row>
+    <row r="77" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R77" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="T77" s="58">
+        <f>SUMIF($R$7:$R$41,$R77,$T$7:$T$41)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R78" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="T78" s="58">
+        <f>SUMIF($R$7:$R$41,$R78,$T$7:$T$41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R80" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="S80" s="68"/>
+      <c r="T80" s="58">
+        <f>SUMIF($R$7:$R$41,$R80,$T$7:$T$41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R81" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="T81" s="58">
+        <f>SUMIF($R$7:$R$41,$R81,$T$7:$T$41)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="18:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R82" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="T82" s="58">
+        <f>SUMIF($R$7:$R$41,$R82,$T$7:$T$41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="18:20" x14ac:dyDescent="0.2">
+      <c r="R83" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="T83" s="58">
+        <f>SUMIF($R$7:$R$41,$R83,$T$7:$T$41)</f>
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added kit quantities to BOM
</commit_message>
<xml_diff>
--- a/hybohat-bom.xlsx
+++ b/hybohat-bom.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rclott/root/files/projs/hybo/eda/public-hybohat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC96E3F-4CF6-204D-B193-EA414625FCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF93E76-B7B3-A646-994A-0F62BCBC793C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51340" yWindow="4720" windowWidth="36180" windowHeight="18400" xr2:uid="{FED97CF3-E78D-5548-AD60-DA55E01ED936}"/>
+    <workbookView xWindow="12660" yWindow="2080" windowWidth="36180" windowHeight="25620" activeTab="1" xr2:uid="{FED97CF3-E78D-5548-AD60-DA55E01ED936}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
-    <sheet name="BOM-COLORS" sheetId="3" r:id="rId2"/>
+    <sheet name="BOM-KIT-VERSION" sheetId="4" r:id="rId2"/>
+    <sheet name="BOM-COLORS" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="hybohat" localSheetId="0">BOM!$C$1:$S$34</definedName>
-    <definedName name="hybohat" localSheetId="1">'BOM-COLORS'!$C$1:$U$38</definedName>
+    <definedName name="hybohat" localSheetId="2">'BOM-COLORS'!$C$1:$U$38</definedName>
+    <definedName name="hybohat" localSheetId="1">'BOM-KIT-VERSION'!$C$1:$O$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{6DED7D30-30E6-8D4C-B5B3-623808C19CE5}" name="hybohat" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+  <connection id="1" xr16:uid="{AFEF9516-31DB-5440-AE1A-DA2F52CC4B6F}" name="hybohat" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
     <textPr sourceFile="/files/projs/hybo/eda/hybohat/hybohat.csv" tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="194">
   <si>
     <t>Ref</t>
   </si>
@@ -638,6 +640,16 @@
   </si>
   <si>
     <t>ASSY</t>
+  </si>
+  <si>
+    <t>F1x19/20</t>
+  </si>
+  <si>
+    <t>Extended
+Qty</t>
+  </si>
+  <si>
+    <t>&lt;=== Total</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1064,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1223,24 +1235,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1329,6 +1323,38 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1353,6 +1379,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hybohat" connectionId="1" xr16:uid="{469F8A43-765B-B449-B3D9-380ED8A10280}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hybohat" connectionId="1" xr16:uid="{DFA7BC69-B964-C64B-B0A0-D1F18BB0752E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1655,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CBE8B4-C17B-C941-A802-EB49C9615736}">
   <dimension ref="B1:W90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,10 +1708,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="81"/>
+      <c r="C1" s="116"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1695,10 +1725,10 @@
       <c r="R1" s="20"/>
     </row>
     <row r="2" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="118"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1712,10 +1742,10 @@
       <c r="R2" s="20"/>
     </row>
     <row r="3" spans="2:23" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78">
+      <c r="B3" s="113">
         <v>44146</v>
       </c>
-      <c r="C3" s="79"/>
+      <c r="C3" s="114"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1848,20 +1878,20 @@
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="116">
+      <c r="B8" s="110">
         <v>2</v>
       </c>
-      <c r="C8" s="117" t="s">
+      <c r="C8" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118">
-        <v>1</v>
-      </c>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112">
+        <v>1</v>
+      </c>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
       <c r="J8" s="15" t="s">
         <v>86</v>
       </c>
@@ -1878,20 +1908,20 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="116">
+      <c r="B9" s="110">
         <v>3</v>
       </c>
-      <c r="C9" s="117" t="s">
+      <c r="C9" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118">
-        <v>1</v>
-      </c>
-      <c r="G9" s="116"/>
-      <c r="H9" s="116"/>
-      <c r="I9" s="116"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112">
+        <v>1</v>
+      </c>
+      <c r="G9" s="110"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
       <c r="J9" s="15" t="s">
         <v>86</v>
       </c>
@@ -1908,20 +1938,20 @@
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="116">
+      <c r="B10" s="110">
         <v>4</v>
       </c>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="111" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="118"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118">
-        <v>1</v>
-      </c>
-      <c r="H10" s="116"/>
-      <c r="I10" s="116"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="112">
+        <v>1</v>
+      </c>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
       <c r="J10" s="15" t="s">
         <v>86</v>
       </c>
@@ -1938,20 +1968,20 @@
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B11" s="116">
+      <c r="B11" s="110">
         <v>5</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="111" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118">
-        <v>1</v>
-      </c>
-      <c r="I11" s="116"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112">
+        <v>1</v>
+      </c>
+      <c r="I11" s="110"/>
       <c r="J11" s="15" t="s">
         <v>86</v>
       </c>
@@ -1968,18 +1998,18 @@
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B12" s="116">
+      <c r="B12" s="110">
         <v>6</v>
       </c>
-      <c r="C12" s="117" t="s">
+      <c r="C12" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118">
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112">
         <v>1</v>
       </c>
       <c r="J12" s="15" t="s">
@@ -2099,229 +2129,229 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="115">
+      <c r="B15" s="109">
         <v>9</v>
       </c>
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="101" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="115">
-        <v>1</v>
-      </c>
-      <c r="E15" s="115">
-        <v>1</v>
-      </c>
-      <c r="F15" s="115">
-        <v>1</v>
-      </c>
-      <c r="G15" s="115">
-        <v>1</v>
-      </c>
-      <c r="H15" s="115">
-        <v>1</v>
-      </c>
-      <c r="I15" s="115">
-        <v>1</v>
-      </c>
-      <c r="J15" s="106" t="s">
+      <c r="D15" s="109">
+        <v>1</v>
+      </c>
+      <c r="E15" s="109">
+        <v>1</v>
+      </c>
+      <c r="F15" s="109">
+        <v>1</v>
+      </c>
+      <c r="G15" s="109">
+        <v>1</v>
+      </c>
+      <c r="H15" s="109">
+        <v>1</v>
+      </c>
+      <c r="I15" s="109">
+        <v>1</v>
+      </c>
+      <c r="J15" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="107"/>
-      <c r="L15" s="108"/>
-      <c r="M15" s="107" t="s">
+      <c r="K15" s="101"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="N15" s="107" t="s">
+      <c r="N15" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="O15" s="106" t="s">
+      <c r="O15" s="100" t="s">
         <v>137</v>
       </c>
-      <c r="P15" s="107" t="s">
+      <c r="P15" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="Q15" s="106" t="str">
+      <c r="Q15" s="100" t="str">
         <f t="shared" ref="Q15:Q37" si="0">MID($P15,1,2)</f>
         <v>M1</v>
       </c>
-      <c r="R15" s="109">
-        <f>VALUE(RIGHT($P15,2))*$D15</f>
+      <c r="R15" s="103">
+        <f t="shared" ref="R15:R20" si="1">VALUE(RIGHT($P15,2))*$D15</f>
         <v>3</v>
       </c>
-      <c r="S15" s="108" t="s">
+      <c r="S15" s="102" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B16" s="115">
+      <c r="B16" s="109">
         <v>10</v>
       </c>
-      <c r="C16" s="107" t="s">
+      <c r="C16" s="101" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="115">
-        <v>1</v>
-      </c>
-      <c r="E16" s="115">
-        <v>1</v>
-      </c>
-      <c r="F16" s="115">
-        <v>1</v>
-      </c>
-      <c r="G16" s="115">
-        <v>1</v>
-      </c>
-      <c r="H16" s="115">
-        <v>1</v>
-      </c>
-      <c r="I16" s="115">
-        <v>1</v>
-      </c>
-      <c r="J16" s="106" t="s">
+      <c r="D16" s="109">
+        <v>1</v>
+      </c>
+      <c r="E16" s="109">
+        <v>1</v>
+      </c>
+      <c r="F16" s="109">
+        <v>1</v>
+      </c>
+      <c r="G16" s="109">
+        <v>1</v>
+      </c>
+      <c r="H16" s="109">
+        <v>1</v>
+      </c>
+      <c r="I16" s="109">
+        <v>1</v>
+      </c>
+      <c r="J16" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="107"/>
-      <c r="L16" s="108"/>
-      <c r="M16" s="107" t="s">
+      <c r="K16" s="101"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="107" t="s">
+      <c r="N16" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="O16" s="106" t="s">
+      <c r="O16" s="100" t="s">
         <v>138</v>
       </c>
-      <c r="P16" s="107" t="s">
+      <c r="P16" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="Q16" s="106" t="str">
+      <c r="Q16" s="100" t="str">
         <f t="shared" si="0"/>
         <v>M1</v>
       </c>
-      <c r="R16" s="109">
-        <f>VALUE(RIGHT($P16,2))*$D16</f>
+      <c r="R16" s="103">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="S16" s="108" t="s">
+      <c r="S16" s="102" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="115">
+      <c r="B17" s="109">
         <v>11</v>
       </c>
-      <c r="C17" s="107" t="s">
+      <c r="C17" s="101" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="115">
-        <v>1</v>
-      </c>
-      <c r="E17" s="115">
-        <v>1</v>
-      </c>
-      <c r="F17" s="115">
-        <v>1</v>
-      </c>
-      <c r="G17" s="115">
-        <v>1</v>
-      </c>
-      <c r="H17" s="115">
-        <v>1</v>
-      </c>
-      <c r="I17" s="115">
-        <v>1</v>
-      </c>
-      <c r="J17" s="106" t="s">
+      <c r="D17" s="109">
+        <v>1</v>
+      </c>
+      <c r="E17" s="109">
+        <v>1</v>
+      </c>
+      <c r="F17" s="109">
+        <v>1</v>
+      </c>
+      <c r="G17" s="109">
+        <v>1</v>
+      </c>
+      <c r="H17" s="109">
+        <v>1</v>
+      </c>
+      <c r="I17" s="109">
+        <v>1</v>
+      </c>
+      <c r="J17" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="107"/>
-      <c r="L17" s="108"/>
-      <c r="M17" s="107" t="s">
+      <c r="K17" s="101"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="N17" s="107" t="s">
+      <c r="N17" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="O17" s="106" t="s">
+      <c r="O17" s="100" t="s">
         <v>139</v>
       </c>
-      <c r="P17" s="107" t="s">
+      <c r="P17" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="Q17" s="106" t="str">
+      <c r="Q17" s="100" t="str">
         <f t="shared" si="0"/>
         <v>M1</v>
       </c>
-      <c r="R17" s="109">
-        <f>VALUE(RIGHT($P17,2))*$D17</f>
+      <c r="R17" s="103">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="S17" s="108" t="s">
+      <c r="S17" s="102" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="115">
+      <c r="B18" s="109">
         <v>12</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="C18" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="115">
-        <v>1</v>
-      </c>
-      <c r="E18" s="115">
-        <v>1</v>
-      </c>
-      <c r="F18" s="115">
-        <v>1</v>
-      </c>
-      <c r="G18" s="115">
-        <v>1</v>
-      </c>
-      <c r="H18" s="115">
-        <v>1</v>
-      </c>
-      <c r="I18" s="115">
-        <v>1</v>
-      </c>
-      <c r="J18" s="106" t="s">
+      <c r="D18" s="109">
+        <v>1</v>
+      </c>
+      <c r="E18" s="109">
+        <v>1</v>
+      </c>
+      <c r="F18" s="109">
+        <v>1</v>
+      </c>
+      <c r="G18" s="109">
+        <v>1</v>
+      </c>
+      <c r="H18" s="109">
+        <v>1</v>
+      </c>
+      <c r="I18" s="109">
+        <v>1</v>
+      </c>
+      <c r="J18" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="K18" s="107"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="107" t="s">
+      <c r="K18" s="101"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="107" t="s">
+      <c r="N18" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="106" t="s">
+      <c r="O18" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="P18" s="107" t="s">
+      <c r="P18" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="Q18" s="106" t="str">
+      <c r="Q18" s="100" t="str">
         <f t="shared" si="0"/>
         <v>M1</v>
       </c>
-      <c r="R18" s="109">
-        <f>VALUE(RIGHT($P18,2))*$D18</f>
+      <c r="R18" s="103">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="S18" s="108" t="s">
+      <c r="S18" s="102" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="7">
+      <c r="B19" s="119">
         <v>13</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="119">
         <v>1</v>
       </c>
       <c r="E19" s="7">
@@ -2361,7 +2391,7 @@
         <v>M2</v>
       </c>
       <c r="R19" s="24">
-        <f>VALUE(RIGHT($P19,2))*$D19</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="S19" s="9" t="s">
@@ -2369,13 +2399,13 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="7">
+      <c r="B20" s="119">
         <v>14</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="119">
         <v>1</v>
       </c>
       <c r="E20" s="7">
@@ -2415,7 +2445,7 @@
         <v>M2</v>
       </c>
       <c r="R20" s="24">
-        <f>VALUE(RIGHT($P20,2))*$D20</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="S20" s="9" t="s">
@@ -2516,98 +2546,98 @@
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="114">
+      <c r="B23" s="108">
         <v>21</v>
       </c>
-      <c r="C23" s="100" t="s">
+      <c r="C23" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="114">
+      <c r="D23" s="108">
         <v>2</v>
       </c>
-      <c r="E23" s="114">
+      <c r="E23" s="108">
         <v>2</v>
       </c>
-      <c r="F23" s="99"/>
-      <c r="G23" s="99"/>
-      <c r="H23" s="99"/>
-      <c r="I23" s="99"/>
-      <c r="J23" s="99" t="s">
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="93"/>
+      <c r="J23" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="100" t="s">
+      <c r="K23" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="L23" s="101" t="s">
+      <c r="L23" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="M23" s="100" t="s">
+      <c r="M23" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="N23" s="100" t="s">
+      <c r="N23" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="99" t="s">
+      <c r="O23" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="P23" s="102" t="s">
+      <c r="P23" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="Q23" s="99" t="str">
+      <c r="Q23" s="93" t="str">
         <f t="shared" si="0"/>
         <v>F1</v>
       </c>
-      <c r="R23" s="103">
-        <f>VALUE(RIGHT($P23,2))*$D23</f>
+      <c r="R23" s="97">
+        <f t="shared" ref="R23:R37" si="2">VALUE(RIGHT($P23,2))*$D23</f>
         <v>38</v>
       </c>
-      <c r="S23" s="101" t="s">
+      <c r="S23" s="95" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="110">
+      <c r="B24" s="104">
         <v>22</v>
       </c>
-      <c r="C24" s="91" t="s">
+      <c r="C24" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="110">
-        <v>1</v>
-      </c>
-      <c r="E24" s="110">
-        <v>1</v>
-      </c>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88" t="s">
+      <c r="D24" s="104">
+        <v>1</v>
+      </c>
+      <c r="E24" s="104">
+        <v>1</v>
+      </c>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K24" s="91"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="91" t="s">
+      <c r="K24" s="85"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N24" s="91" t="s">
+      <c r="N24" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="O24" s="88" t="s">
+      <c r="O24" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="P24" s="91" t="s">
+      <c r="P24" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="Q24" s="88" t="str">
+      <c r="Q24" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R24" s="93">
-        <f>VALUE(RIGHT($P24,2))*$D24</f>
+      <c r="R24" s="87">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S24" s="92" t="s">
+      <c r="S24" s="86" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2654,7 +2684,7 @@
         <v>F2</v>
       </c>
       <c r="R25" s="24">
-        <f>VALUE(RIGHT($P25,2))*$D25</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="S25" s="9" t="s">
@@ -2696,15 +2726,15 @@
       <c r="O26" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="P26" s="104" t="s">
+      <c r="P26" s="98" t="s">
         <v>63</v>
       </c>
       <c r="Q26" s="25" t="str">
         <f t="shared" si="0"/>
         <v>F1</v>
       </c>
-      <c r="R26" s="105">
-        <f>VALUE(RIGHT($P26,2))*$D26</f>
+      <c r="R26" s="99">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="S26" s="74" t="s">
@@ -2754,7 +2784,7 @@
         <v>F2</v>
       </c>
       <c r="R27" s="24">
-        <f>VALUE(RIGHT($P27,2))*$D27</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="S27" s="9" t="s">
@@ -2762,462 +2792,462 @@
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="110">
+      <c r="B28" s="104">
         <v>26</v>
       </c>
-      <c r="C28" s="91" t="s">
+      <c r="C28" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="110">
-        <v>1</v>
-      </c>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
-      <c r="H28" s="110">
-        <v>1</v>
-      </c>
-      <c r="I28" s="110"/>
-      <c r="J28" s="88" t="s">
+      <c r="D28" s="104">
+        <v>1</v>
+      </c>
+      <c r="E28" s="104"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="104"/>
+      <c r="H28" s="104">
+        <v>1</v>
+      </c>
+      <c r="I28" s="104"/>
+      <c r="J28" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K28" s="91"/>
-      <c r="L28" s="92"/>
-      <c r="M28" s="91" t="s">
+      <c r="K28" s="85"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="N28" s="91" t="s">
+      <c r="N28" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="O28" s="88" t="s">
+      <c r="O28" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="P28" s="91" t="s">
+      <c r="P28" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="Q28" s="88" t="str">
+      <c r="Q28" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R28" s="93">
-        <f>VALUE(RIGHT($P28,2))*$D28</f>
+      <c r="R28" s="87">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S28" s="92" t="s">
+      <c r="S28" s="86" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="110">
+      <c r="B29" s="104">
         <v>27</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="110">
-        <v>1</v>
-      </c>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
-      <c r="G29" s="110"/>
-      <c r="H29" s="110">
-        <v>1</v>
-      </c>
-      <c r="I29" s="110"/>
-      <c r="J29" s="88" t="s">
+      <c r="D29" s="104">
+        <v>1</v>
+      </c>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104">
+        <v>1</v>
+      </c>
+      <c r="I29" s="104"/>
+      <c r="J29" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K29" s="91"/>
-      <c r="L29" s="92"/>
-      <c r="M29" s="91" t="s">
+      <c r="K29" s="85"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="N29" s="91" t="s">
+      <c r="N29" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="O29" s="88" t="s">
+      <c r="O29" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="P29" s="91" t="s">
+      <c r="P29" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Q29" s="88" t="str">
+      <c r="Q29" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R29" s="93">
-        <f>VALUE(RIGHT($P29,2))*$D29</f>
+      <c r="R29" s="87">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S29" s="92" t="s">
+      <c r="S29" s="86" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="110">
+      <c r="B30" s="104">
         <v>28</v>
       </c>
-      <c r="C30" s="91" t="s">
+      <c r="C30" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="110">
-        <v>1</v>
-      </c>
-      <c r="E30" s="110"/>
-      <c r="F30" s="110"/>
-      <c r="G30" s="110"/>
-      <c r="H30" s="110">
-        <v>1</v>
-      </c>
-      <c r="I30" s="110"/>
-      <c r="J30" s="88" t="s">
+      <c r="D30" s="104">
+        <v>1</v>
+      </c>
+      <c r="E30" s="104"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="104">
+        <v>1</v>
+      </c>
+      <c r="I30" s="104"/>
+      <c r="J30" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K30" s="91"/>
-      <c r="L30" s="92"/>
-      <c r="M30" s="91" t="s">
+      <c r="K30" s="85"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="N30" s="91" t="s">
+      <c r="N30" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="O30" s="88" t="s">
+      <c r="O30" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="P30" s="91" t="s">
+      <c r="P30" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Q30" s="88" t="str">
+      <c r="Q30" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R30" s="93">
-        <f>VALUE(RIGHT($P30,2))*$D30</f>
+      <c r="R30" s="87">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S30" s="92" t="s">
+      <c r="S30" s="86" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="110">
+      <c r="B31" s="104">
         <v>29</v>
       </c>
-      <c r="C31" s="91" t="s">
+      <c r="C31" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="110">
-        <v>1</v>
-      </c>
-      <c r="E31" s="110"/>
-      <c r="F31" s="110"/>
-      <c r="G31" s="110"/>
-      <c r="H31" s="110"/>
-      <c r="I31" s="110">
-        <v>1</v>
-      </c>
-      <c r="J31" s="88" t="s">
+      <c r="D31" s="104">
+        <v>1</v>
+      </c>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104">
+        <v>1</v>
+      </c>
+      <c r="J31" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K31" s="91"/>
-      <c r="L31" s="92"/>
-      <c r="M31" s="91" t="s">
+      <c r="K31" s="85"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="N31" s="91" t="s">
+      <c r="N31" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="O31" s="88" t="s">
+      <c r="O31" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P31" s="95" t="s">
+      <c r="P31" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="Q31" s="88" t="str">
+      <c r="Q31" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R31" s="93">
-        <f>VALUE(RIGHT($P31,2))*$D31</f>
+      <c r="R31" s="87">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S31" s="92" t="s">
+      <c r="S31" s="86" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="110">
+      <c r="B32" s="104">
         <v>30</v>
       </c>
-      <c r="C32" s="91" t="s">
+      <c r="C32" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="110">
-        <v>1</v>
-      </c>
-      <c r="E32" s="110"/>
-      <c r="F32" s="110"/>
-      <c r="G32" s="110"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110">
-        <v>1</v>
-      </c>
-      <c r="J32" s="88" t="s">
+      <c r="D32" s="104">
+        <v>1</v>
+      </c>
+      <c r="E32" s="104"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104">
+        <v>1</v>
+      </c>
+      <c r="J32" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K32" s="91"/>
-      <c r="L32" s="92"/>
-      <c r="M32" s="91" t="s">
+      <c r="K32" s="85"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="N32" s="91" t="s">
+      <c r="N32" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="O32" s="88" t="s">
+      <c r="O32" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P32" s="95" t="s">
+      <c r="P32" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="Q32" s="88" t="str">
+      <c r="Q32" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R32" s="93">
-        <f>VALUE(RIGHT($P32,2))*$D32</f>
+      <c r="R32" s="87">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="S32" s="92" t="s">
+      <c r="S32" s="86" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B33" s="110">
+      <c r="B33" s="104">
         <v>31</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="110">
-        <v>1</v>
-      </c>
-      <c r="E33" s="110"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="110">
-        <v>1</v>
-      </c>
-      <c r="J33" s="88" t="s">
+      <c r="D33" s="104">
+        <v>1</v>
+      </c>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104">
+        <v>1</v>
+      </c>
+      <c r="J33" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K33" s="91"/>
-      <c r="L33" s="92"/>
-      <c r="M33" s="91" t="s">
+      <c r="K33" s="85"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="N33" s="91" t="s">
+      <c r="N33" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="O33" s="88" t="s">
+      <c r="O33" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P33" s="95" t="s">
+      <c r="P33" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="Q33" s="88" t="str">
+      <c r="Q33" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R33" s="93">
-        <f>VALUE(RIGHT($P33,2))*$D33</f>
+      <c r="R33" s="87">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="S33" s="92" t="s">
+      <c r="S33" s="86" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="110">
+      <c r="B34" s="104">
         <v>32</v>
       </c>
-      <c r="C34" s="91" t="s">
+      <c r="C34" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="110">
-        <v>1</v>
-      </c>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="110">
-        <v>1</v>
-      </c>
-      <c r="J34" s="88" t="s">
+      <c r="D34" s="104">
+        <v>1</v>
+      </c>
+      <c r="E34" s="104"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104">
+        <v>1</v>
+      </c>
+      <c r="J34" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K34" s="91"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="91" t="s">
+      <c r="K34" s="85"/>
+      <c r="L34" s="86"/>
+      <c r="M34" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="N34" s="91" t="s">
+      <c r="N34" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="O34" s="88" t="s">
+      <c r="O34" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P34" s="95" t="s">
+      <c r="P34" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="Q34" s="88" t="str">
+      <c r="Q34" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R34" s="93">
-        <f>VALUE(RIGHT($P34,2))*$D34</f>
+      <c r="R34" s="87">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="S34" s="92" t="s">
+      <c r="S34" s="86" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B35" s="110">
+      <c r="B35" s="104">
         <v>33</v>
       </c>
-      <c r="C35" s="91" t="s">
+      <c r="C35" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="110">
-        <v>1</v>
-      </c>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="110">
-        <v>1</v>
-      </c>
-      <c r="J35" s="88" t="s">
+      <c r="D35" s="104">
+        <v>1</v>
+      </c>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104">
+        <v>1</v>
+      </c>
+      <c r="J35" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="91"/>
-      <c r="L35" s="92"/>
-      <c r="M35" s="91" t="s">
+      <c r="K35" s="85"/>
+      <c r="L35" s="86"/>
+      <c r="M35" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="91" t="s">
+      <c r="N35" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="O35" s="88" t="s">
+      <c r="O35" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P35" s="91" t="s">
+      <c r="P35" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="Q35" s="88" t="str">
+      <c r="Q35" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R35" s="93">
-        <f>VALUE(RIGHT($P35,2))*$D35</f>
+      <c r="R35" s="87">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="S35" s="92" t="s">
+      <c r="S35" s="86" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B36" s="110">
+      <c r="B36" s="104">
         <v>34</v>
       </c>
-      <c r="C36" s="91" t="s">
+      <c r="C36" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="110">
-        <v>1</v>
-      </c>
-      <c r="E36" s="110"/>
-      <c r="F36" s="110"/>
-      <c r="G36" s="110"/>
-      <c r="H36" s="110"/>
-      <c r="I36" s="110">
-        <v>1</v>
-      </c>
-      <c r="J36" s="88" t="s">
+      <c r="D36" s="104">
+        <v>1</v>
+      </c>
+      <c r="E36" s="104"/>
+      <c r="F36" s="104"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="104">
+        <v>1</v>
+      </c>
+      <c r="J36" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K36" s="91"/>
-      <c r="L36" s="92"/>
-      <c r="M36" s="91" t="s">
+      <c r="K36" s="85"/>
+      <c r="L36" s="86"/>
+      <c r="M36" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="N36" s="91" t="s">
+      <c r="N36" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="O36" s="88" t="s">
+      <c r="O36" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P36" s="95" t="s">
+      <c r="P36" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="Q36" s="88" t="str">
+      <c r="Q36" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R36" s="93">
-        <f>VALUE(RIGHT($P36,2))*$D36</f>
+      <c r="R36" s="87">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S36" s="92" t="s">
+      <c r="S36" s="86" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B37" s="110">
+      <c r="B37" s="104">
         <v>35</v>
       </c>
-      <c r="C37" s="91" t="s">
+      <c r="C37" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="110">
-        <v>1</v>
-      </c>
-      <c r="E37" s="110"/>
-      <c r="F37" s="110"/>
-      <c r="G37" s="110"/>
-      <c r="H37" s="110"/>
-      <c r="I37" s="110">
-        <v>1</v>
-      </c>
-      <c r="J37" s="88" t="s">
+      <c r="D37" s="104">
+        <v>1</v>
+      </c>
+      <c r="E37" s="104"/>
+      <c r="F37" s="104"/>
+      <c r="G37" s="104"/>
+      <c r="H37" s="104"/>
+      <c r="I37" s="104">
+        <v>1</v>
+      </c>
+      <c r="J37" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K37" s="91"/>
-      <c r="L37" s="92"/>
-      <c r="M37" s="91" t="s">
+      <c r="K37" s="85"/>
+      <c r="L37" s="86"/>
+      <c r="M37" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="N37" s="91" t="s">
+      <c r="N37" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="O37" s="88" t="s">
+      <c r="O37" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="P37" s="95" t="s">
+      <c r="P37" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="Q37" s="88" t="str">
+      <c r="Q37" s="82" t="str">
         <f t="shared" si="0"/>
         <v>M2</v>
       </c>
-      <c r="R37" s="93">
-        <f>VALUE(RIGHT($P37,2))*$D37</f>
+      <c r="R37" s="87">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="S37" s="92" t="s">
+      <c r="S37" s="86" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3262,171 +3292,171 @@
       </c>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="111">
+      <c r="B41" s="105">
         <v>91</v>
       </c>
-      <c r="C41" s="100" t="s">
+      <c r="C41" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="99">
+      <c r="D41" s="93">
         <v>2</v>
       </c>
-      <c r="E41" s="99">
+      <c r="E41" s="93">
         <v>2</v>
       </c>
-      <c r="F41" s="99">
+      <c r="F41" s="93">
         <v>2</v>
       </c>
-      <c r="G41" s="99">
+      <c r="G41" s="93">
         <v>2</v>
       </c>
-      <c r="H41" s="99">
+      <c r="H41" s="93">
         <v>2</v>
       </c>
-      <c r="I41" s="99">
+      <c r="I41" s="93">
         <v>2</v>
       </c>
-      <c r="J41" s="99" t="s">
+      <c r="J41" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="K41" s="100" t="s">
+      <c r="K41" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="L41" s="101" t="s">
+      <c r="L41" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="M41" s="100"/>
-      <c r="N41" s="100"/>
-      <c r="O41" s="99" t="s">
+      <c r="M41" s="94"/>
+      <c r="N41" s="94"/>
+      <c r="O41" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="P41" s="102" t="s">
+      <c r="P41" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="Q41" s="99"/>
-      <c r="R41" s="103"/>
-      <c r="S41" s="101" t="s">
+      <c r="Q41" s="93"/>
+      <c r="R41" s="97"/>
+      <c r="S41" s="95" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="113">
+      <c r="B42" s="107">
         <v>92</v>
       </c>
-      <c r="C42" s="107" t="s">
+      <c r="C42" s="101" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="106">
-        <v>1</v>
-      </c>
-      <c r="E42" s="106">
-        <v>1</v>
-      </c>
-      <c r="F42" s="106">
-        <v>1</v>
-      </c>
-      <c r="G42" s="106">
-        <v>1</v>
-      </c>
-      <c r="H42" s="106">
-        <v>1</v>
-      </c>
-      <c r="I42" s="106">
-        <v>1</v>
-      </c>
-      <c r="J42" s="106" t="s">
+      <c r="D42" s="100">
+        <v>1</v>
+      </c>
+      <c r="E42" s="100">
+        <v>1</v>
+      </c>
+      <c r="F42" s="100">
+        <v>1</v>
+      </c>
+      <c r="G42" s="100">
+        <v>1</v>
+      </c>
+      <c r="H42" s="100">
+        <v>1</v>
+      </c>
+      <c r="I42" s="100">
+        <v>1</v>
+      </c>
+      <c r="J42" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="K42" s="107" t="s">
+      <c r="K42" s="101" t="s">
         <v>125</v>
       </c>
-      <c r="L42" s="108" t="s">
+      <c r="L42" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="M42" s="107"/>
-      <c r="N42" s="107"/>
-      <c r="O42" s="106" t="s">
+      <c r="M42" s="101"/>
+      <c r="N42" s="101"/>
+      <c r="O42" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="P42" s="106" t="s">
+      <c r="P42" s="100" t="s">
         <v>184</v>
       </c>
-      <c r="Q42" s="106"/>
-      <c r="R42" s="109"/>
-      <c r="S42" s="107" t="s">
+      <c r="Q42" s="100"/>
+      <c r="R42" s="103"/>
+      <c r="S42" s="101" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="112">
+      <c r="B43" s="106">
         <v>93</v>
       </c>
-      <c r="C43" s="91" t="s">
+      <c r="C43" s="85" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="88">
+      <c r="D43" s="82">
         <v>4</v>
       </c>
-      <c r="E43" s="88">
+      <c r="E43" s="82">
         <v>4</v>
       </c>
-      <c r="F43" s="88">
+      <c r="F43" s="82">
         <v>4</v>
       </c>
-      <c r="G43" s="88">
+      <c r="G43" s="82">
         <v>4</v>
       </c>
-      <c r="H43" s="88">
+      <c r="H43" s="82">
         <v>4</v>
       </c>
-      <c r="I43" s="88">
+      <c r="I43" s="82">
         <v>4</v>
       </c>
-      <c r="J43" s="88" t="s">
+      <c r="J43" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="K43" s="91" t="s">
+      <c r="K43" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="L43" s="92" t="s">
+      <c r="L43" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="M43" s="91"/>
-      <c r="N43" s="91"/>
-      <c r="O43" s="88" t="s">
+      <c r="M43" s="85"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="P43" s="88" t="s">
+      <c r="P43" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="Q43" s="88"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="91" t="s">
+      <c r="Q43" s="82"/>
+      <c r="R43" s="87"/>
+      <c r="S43" s="85" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="46" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="Q47" s="96" t="s">
+      <c r="Q47" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="R47" s="94">
+      <c r="R47" s="88">
         <f>SUMIF($Q$7:$Q$37,$Q47,$R$7:$R$37)</f>
         <v>16</v>
       </c>
-      <c r="S47" s="97" t="s">
+      <c r="S47" s="91" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="48" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="Q48" s="98" t="s">
+      <c r="Q48" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="R48" s="89">
+      <c r="R48" s="83">
         <f>SUMIF($Q$7:$Q$37,$Q48,$R$7:$R$37)</f>
         <v>118</v>
       </c>
-      <c r="S48" s="90" t="s">
+      <c r="S48" s="84" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3461,541 +3491,541 @@
       <c r="S54" s="70"/>
     </row>
     <row r="55" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="84"/>
-      <c r="G55" s="84"/>
-      <c r="H55" s="84"/>
-      <c r="I55" s="84"/>
-      <c r="J55" s="84"/>
-      <c r="L55" s="85"/>
-      <c r="O55" s="84"/>
+      <c r="B55" s="78"/>
+      <c r="D55" s="78"/>
+      <c r="E55" s="78"/>
+      <c r="F55" s="78"/>
+      <c r="G55" s="78"/>
+      <c r="H55" s="78"/>
+      <c r="I55" s="78"/>
+      <c r="J55" s="78"/>
+      <c r="L55" s="79"/>
+      <c r="O55" s="78"/>
       <c r="Q55" s="68"/>
       <c r="R55" s="69"/>
       <c r="S55" s="70"/>
     </row>
     <row r="56" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="84"/>
-      <c r="D56" s="84"/>
-      <c r="E56" s="84"/>
-      <c r="F56" s="84"/>
-      <c r="G56" s="84"/>
-      <c r="H56" s="84"/>
-      <c r="I56" s="84"/>
-      <c r="J56" s="84"/>
-      <c r="L56" s="85"/>
-      <c r="O56" s="84"/>
+      <c r="B56" s="78"/>
+      <c r="D56" s="78"/>
+      <c r="E56" s="78"/>
+      <c r="F56" s="78"/>
+      <c r="G56" s="78"/>
+      <c r="H56" s="78"/>
+      <c r="I56" s="78"/>
+      <c r="J56" s="78"/>
+      <c r="L56" s="79"/>
+      <c r="O56" s="78"/>
       <c r="Q56" s="68"/>
       <c r="R56" s="69"/>
       <c r="S56" s="70"/>
     </row>
     <row r="57" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="84"/>
-      <c r="D57" s="84"/>
-      <c r="E57" s="84"/>
-      <c r="F57" s="84"/>
-      <c r="G57" s="84"/>
-      <c r="H57" s="84"/>
-      <c r="I57" s="84"/>
-      <c r="J57" s="84"/>
-      <c r="L57" s="85"/>
-      <c r="O57" s="84"/>
+      <c r="B57" s="78"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="78"/>
+      <c r="F57" s="78"/>
+      <c r="G57" s="78"/>
+      <c r="H57" s="78"/>
+      <c r="I57" s="78"/>
+      <c r="J57" s="78"/>
+      <c r="L57" s="79"/>
+      <c r="O57" s="78"/>
       <c r="Q57" s="68"/>
       <c r="R57" s="69"/>
       <c r="S57" s="70"/>
     </row>
     <row r="58" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="84"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="84"/>
-      <c r="F58" s="84"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="84"/>
-      <c r="I58" s="84"/>
-      <c r="J58" s="84"/>
-      <c r="L58" s="85"/>
-      <c r="O58" s="84"/>
+      <c r="B58" s="78"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="78"/>
+      <c r="F58" s="78"/>
+      <c r="G58" s="78"/>
+      <c r="H58" s="78"/>
+      <c r="I58" s="78"/>
+      <c r="J58" s="78"/>
+      <c r="L58" s="79"/>
+      <c r="O58" s="78"/>
       <c r="Q58" s="68"/>
       <c r="R58" s="69"/>
-      <c r="S58" s="87"/>
+      <c r="S58" s="81"/>
     </row>
     <row r="59" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="84"/>
-      <c r="D59" s="84"/>
-      <c r="E59" s="84"/>
-      <c r="F59" s="84"/>
-      <c r="G59" s="84"/>
-      <c r="H59" s="84"/>
-      <c r="I59" s="84"/>
-      <c r="J59" s="84"/>
-      <c r="L59" s="85"/>
-      <c r="O59" s="84"/>
+      <c r="B59" s="78"/>
+      <c r="D59" s="78"/>
+      <c r="E59" s="78"/>
+      <c r="F59" s="78"/>
+      <c r="G59" s="78"/>
+      <c r="H59" s="78"/>
+      <c r="I59" s="78"/>
+      <c r="J59" s="78"/>
+      <c r="L59" s="79"/>
+      <c r="O59" s="78"/>
       <c r="Q59" s="68"/>
       <c r="R59" s="69"/>
-      <c r="S59" s="87"/>
+      <c r="S59" s="81"/>
     </row>
     <row r="60" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="84"/>
-      <c r="D60" s="84"/>
-      <c r="E60" s="84"/>
-      <c r="F60" s="84"/>
-      <c r="G60" s="84"/>
-      <c r="H60" s="84"/>
-      <c r="I60" s="84"/>
-      <c r="J60" s="84"/>
-      <c r="L60" s="85"/>
-      <c r="O60" s="84"/>
+      <c r="B60" s="78"/>
+      <c r="D60" s="78"/>
+      <c r="E60" s="78"/>
+      <c r="F60" s="78"/>
+      <c r="G60" s="78"/>
+      <c r="H60" s="78"/>
+      <c r="I60" s="78"/>
+      <c r="J60" s="78"/>
+      <c r="L60" s="79"/>
+      <c r="O60" s="78"/>
       <c r="Q60" s="68"/>
       <c r="R60" s="69"/>
       <c r="S60" s="70"/>
     </row>
     <row r="61" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="84"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="84"/>
-      <c r="F61" s="84"/>
-      <c r="G61" s="84"/>
-      <c r="H61" s="84"/>
-      <c r="I61" s="84"/>
-      <c r="J61" s="84"/>
-      <c r="L61" s="85"/>
-      <c r="O61" s="84"/>
+      <c r="B61" s="78"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="78"/>
+      <c r="F61" s="78"/>
+      <c r="G61" s="78"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="78"/>
+      <c r="J61" s="78"/>
+      <c r="L61" s="79"/>
+      <c r="O61" s="78"/>
       <c r="Q61" s="68"/>
       <c r="R61" s="69"/>
       <c r="S61" s="70"/>
     </row>
     <row r="62" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="84"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="84"/>
-      <c r="F62" s="84"/>
-      <c r="G62" s="84"/>
-      <c r="H62" s="84"/>
-      <c r="I62" s="84"/>
-      <c r="J62" s="84"/>
-      <c r="L62" s="85"/>
-      <c r="O62" s="84"/>
+      <c r="B62" s="78"/>
+      <c r="D62" s="78"/>
+      <c r="E62" s="78"/>
+      <c r="F62" s="78"/>
+      <c r="G62" s="78"/>
+      <c r="H62" s="78"/>
+      <c r="I62" s="78"/>
+      <c r="J62" s="78"/>
+      <c r="L62" s="79"/>
+      <c r="O62" s="78"/>
       <c r="Q62" s="68"/>
       <c r="R62" s="69"/>
       <c r="S62" s="70"/>
     </row>
     <row r="63" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="84"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="84"/>
-      <c r="F63" s="84"/>
-      <c r="G63" s="84"/>
-      <c r="H63" s="84"/>
-      <c r="I63" s="84"/>
-      <c r="J63" s="84"/>
-      <c r="L63" s="85"/>
-      <c r="O63" s="84"/>
+      <c r="B63" s="78"/>
+      <c r="D63" s="78"/>
+      <c r="E63" s="78"/>
+      <c r="F63" s="78"/>
+      <c r="G63" s="78"/>
+      <c r="H63" s="78"/>
+      <c r="I63" s="78"/>
+      <c r="J63" s="78"/>
+      <c r="L63" s="79"/>
+      <c r="O63" s="78"/>
       <c r="Q63" s="68"/>
       <c r="R63" s="69"/>
       <c r="S63" s="70"/>
     </row>
     <row r="64" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="84"/>
-      <c r="D64" s="84"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="84"/>
-      <c r="G64" s="84"/>
-      <c r="H64" s="84"/>
-      <c r="I64" s="84"/>
-      <c r="J64" s="84"/>
-      <c r="L64" s="85"/>
-      <c r="O64" s="84"/>
+      <c r="B64" s="78"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="78"/>
+      <c r="H64" s="78"/>
+      <c r="I64" s="78"/>
+      <c r="J64" s="78"/>
+      <c r="L64" s="79"/>
+      <c r="O64" s="78"/>
       <c r="Q64" s="68"/>
       <c r="R64" s="69"/>
       <c r="S64" s="70"/>
     </row>
     <row r="65" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="84"/>
-      <c r="D65" s="84"/>
-      <c r="E65" s="84"/>
-      <c r="F65" s="84"/>
-      <c r="G65" s="84"/>
-      <c r="H65" s="84"/>
-      <c r="I65" s="84"/>
-      <c r="J65" s="84"/>
-      <c r="L65" s="85"/>
-      <c r="O65" s="84"/>
+      <c r="B65" s="78"/>
+      <c r="D65" s="78"/>
+      <c r="E65" s="78"/>
+      <c r="F65" s="78"/>
+      <c r="G65" s="78"/>
+      <c r="H65" s="78"/>
+      <c r="I65" s="78"/>
+      <c r="J65" s="78"/>
+      <c r="L65" s="79"/>
+      <c r="O65" s="78"/>
       <c r="Q65" s="68"/>
       <c r="R65" s="69"/>
       <c r="S65" s="70"/>
     </row>
     <row r="66" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="84"/>
-      <c r="D66" s="84"/>
-      <c r="E66" s="84"/>
-      <c r="F66" s="84"/>
-      <c r="G66" s="84"/>
-      <c r="H66" s="84"/>
-      <c r="I66" s="84"/>
-      <c r="J66" s="84"/>
-      <c r="L66" s="85"/>
-      <c r="O66" s="84"/>
+      <c r="B66" s="78"/>
+      <c r="D66" s="78"/>
+      <c r="E66" s="78"/>
+      <c r="F66" s="78"/>
+      <c r="G66" s="78"/>
+      <c r="H66" s="78"/>
+      <c r="I66" s="78"/>
+      <c r="J66" s="78"/>
+      <c r="L66" s="79"/>
+      <c r="O66" s="78"/>
       <c r="Q66" s="68"/>
       <c r="R66" s="69"/>
       <c r="S66" s="70"/>
     </row>
     <row r="67" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="84"/>
-      <c r="D67" s="84"/>
-      <c r="E67" s="84"/>
-      <c r="F67" s="84"/>
-      <c r="G67" s="84"/>
-      <c r="H67" s="84"/>
-      <c r="I67" s="84"/>
-      <c r="J67" s="84"/>
-      <c r="L67" s="85"/>
-      <c r="O67" s="84"/>
+      <c r="B67" s="78"/>
+      <c r="D67" s="78"/>
+      <c r="E67" s="78"/>
+      <c r="F67" s="78"/>
+      <c r="G67" s="78"/>
+      <c r="H67" s="78"/>
+      <c r="I67" s="78"/>
+      <c r="J67" s="78"/>
+      <c r="L67" s="79"/>
+      <c r="O67" s="78"/>
       <c r="Q67" s="68"/>
       <c r="R67" s="69"/>
       <c r="S67" s="70"/>
     </row>
     <row r="68" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="84"/>
-      <c r="D68" s="84"/>
-      <c r="E68" s="84"/>
-      <c r="F68" s="84"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="84"/>
-      <c r="I68" s="84"/>
-      <c r="J68" s="84"/>
-      <c r="L68" s="85"/>
-      <c r="O68" s="84"/>
+      <c r="B68" s="78"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="78"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
+      <c r="I68" s="78"/>
+      <c r="J68" s="78"/>
+      <c r="L68" s="79"/>
+      <c r="O68" s="78"/>
       <c r="Q68" s="68"/>
       <c r="R68" s="69"/>
       <c r="S68" s="70"/>
     </row>
     <row r="69" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="84"/>
-      <c r="D69" s="84"/>
-      <c r="E69" s="84"/>
-      <c r="F69" s="84"/>
-      <c r="G69" s="84"/>
-      <c r="H69" s="84"/>
-      <c r="I69" s="84"/>
-      <c r="J69" s="84"/>
-      <c r="L69" s="85"/>
-      <c r="O69" s="84"/>
+      <c r="B69" s="78"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="78"/>
+      <c r="F69" s="78"/>
+      <c r="G69" s="78"/>
+      <c r="H69" s="78"/>
+      <c r="I69" s="78"/>
+      <c r="J69" s="78"/>
+      <c r="L69" s="79"/>
+      <c r="O69" s="78"/>
       <c r="Q69" s="68"/>
       <c r="R69" s="69"/>
       <c r="S69" s="70"/>
     </row>
     <row r="70" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="84"/>
-      <c r="D70" s="84"/>
-      <c r="E70" s="84"/>
-      <c r="F70" s="84"/>
-      <c r="G70" s="84"/>
-      <c r="H70" s="84"/>
-      <c r="I70" s="84"/>
-      <c r="J70" s="84"/>
-      <c r="L70" s="85"/>
-      <c r="O70" s="84"/>
+      <c r="B70" s="78"/>
+      <c r="D70" s="78"/>
+      <c r="E70" s="78"/>
+      <c r="F70" s="78"/>
+      <c r="G70" s="78"/>
+      <c r="H70" s="78"/>
+      <c r="I70" s="78"/>
+      <c r="J70" s="78"/>
+      <c r="L70" s="79"/>
+      <c r="O70" s="78"/>
       <c r="Q70" s="68"/>
       <c r="R70" s="69"/>
       <c r="S70" s="70"/>
     </row>
     <row r="71" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="84"/>
-      <c r="D71" s="84"/>
-      <c r="E71" s="84"/>
-      <c r="F71" s="84"/>
-      <c r="G71" s="84"/>
-      <c r="H71" s="84"/>
-      <c r="I71" s="84"/>
-      <c r="J71" s="84"/>
-      <c r="L71" s="85"/>
-      <c r="O71" s="84"/>
+      <c r="B71" s="78"/>
+      <c r="D71" s="78"/>
+      <c r="E71" s="78"/>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
+      <c r="I71" s="78"/>
+      <c r="J71" s="78"/>
+      <c r="L71" s="79"/>
+      <c r="O71" s="78"/>
       <c r="Q71" s="68"/>
       <c r="R71" s="69"/>
       <c r="S71" s="70"/>
     </row>
     <row r="72" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="84"/>
-      <c r="D72" s="84"/>
-      <c r="E72" s="84"/>
-      <c r="F72" s="84"/>
-      <c r="G72" s="84"/>
-      <c r="H72" s="84"/>
-      <c r="I72" s="84"/>
-      <c r="J72" s="84"/>
-      <c r="L72" s="85"/>
-      <c r="O72" s="84"/>
+      <c r="B72" s="78"/>
+      <c r="D72" s="78"/>
+      <c r="E72" s="78"/>
+      <c r="F72" s="78"/>
+      <c r="G72" s="78"/>
+      <c r="H72" s="78"/>
+      <c r="I72" s="78"/>
+      <c r="J72" s="78"/>
+      <c r="L72" s="79"/>
+      <c r="O72" s="78"/>
       <c r="Q72" s="68"/>
       <c r="R72" s="69"/>
       <c r="S72" s="70"/>
     </row>
     <row r="73" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="84"/>
-      <c r="D73" s="84"/>
-      <c r="E73" s="84"/>
-      <c r="F73" s="84"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="84"/>
-      <c r="I73" s="84"/>
-      <c r="J73" s="84"/>
-      <c r="L73" s="85"/>
-      <c r="O73" s="84"/>
+      <c r="B73" s="78"/>
+      <c r="D73" s="78"/>
+      <c r="E73" s="78"/>
+      <c r="F73" s="78"/>
+      <c r="G73" s="78"/>
+      <c r="H73" s="78"/>
+      <c r="I73" s="78"/>
+      <c r="J73" s="78"/>
+      <c r="L73" s="79"/>
+      <c r="O73" s="78"/>
       <c r="Q73" s="68"/>
       <c r="R73" s="69"/>
       <c r="S73" s="70"/>
     </row>
     <row r="74" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="84"/>
-      <c r="D74" s="84"/>
-      <c r="E74" s="84"/>
-      <c r="F74" s="84"/>
-      <c r="G74" s="84"/>
-      <c r="H74" s="84"/>
-      <c r="I74" s="84"/>
-      <c r="J74" s="84"/>
-      <c r="L74" s="85"/>
-      <c r="O74" s="84"/>
+      <c r="B74" s="78"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="78"/>
+      <c r="G74" s="78"/>
+      <c r="H74" s="78"/>
+      <c r="I74" s="78"/>
+      <c r="J74" s="78"/>
+      <c r="L74" s="79"/>
+      <c r="O74" s="78"/>
       <c r="Q74" s="68"/>
       <c r="R74" s="69"/>
       <c r="S74" s="70"/>
     </row>
     <row r="75" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="84"/>
-      <c r="D75" s="84"/>
-      <c r="E75" s="84"/>
-      <c r="F75" s="84"/>
-      <c r="G75" s="84"/>
-      <c r="H75" s="84"/>
-      <c r="I75" s="84"/>
-      <c r="J75" s="84"/>
-      <c r="L75" s="85"/>
-      <c r="O75" s="84"/>
+      <c r="B75" s="78"/>
+      <c r="D75" s="78"/>
+      <c r="E75" s="78"/>
+      <c r="F75" s="78"/>
+      <c r="G75" s="78"/>
+      <c r="H75" s="78"/>
+      <c r="I75" s="78"/>
+      <c r="J75" s="78"/>
+      <c r="L75" s="79"/>
+      <c r="O75" s="78"/>
       <c r="Q75" s="68"/>
       <c r="R75" s="69"/>
       <c r="S75" s="70"/>
     </row>
     <row r="76" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="84"/>
-      <c r="D76" s="84"/>
-      <c r="E76" s="84"/>
-      <c r="F76" s="84"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="84"/>
-      <c r="I76" s="84"/>
-      <c r="J76" s="84"/>
-      <c r="L76" s="85"/>
-      <c r="O76" s="84"/>
+      <c r="B76" s="78"/>
+      <c r="D76" s="78"/>
+      <c r="E76" s="78"/>
+      <c r="F76" s="78"/>
+      <c r="G76" s="78"/>
+      <c r="H76" s="78"/>
+      <c r="I76" s="78"/>
+      <c r="J76" s="78"/>
+      <c r="L76" s="79"/>
+      <c r="O76" s="78"/>
       <c r="Q76" s="68"/>
       <c r="R76" s="69"/>
       <c r="S76" s="70"/>
     </row>
     <row r="77" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="84"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="84"/>
-      <c r="F77" s="84"/>
-      <c r="G77" s="84"/>
-      <c r="H77" s="84"/>
-      <c r="I77" s="84"/>
-      <c r="J77" s="84"/>
-      <c r="L77" s="85"/>
-      <c r="O77" s="84"/>
+      <c r="B77" s="78"/>
+      <c r="D77" s="78"/>
+      <c r="E77" s="78"/>
+      <c r="F77" s="78"/>
+      <c r="G77" s="78"/>
+      <c r="H77" s="78"/>
+      <c r="I77" s="78"/>
+      <c r="J77" s="78"/>
+      <c r="L77" s="79"/>
+      <c r="O77" s="78"/>
       <c r="Q77" s="68"/>
       <c r="R77" s="69"/>
       <c r="S77" s="70"/>
     </row>
     <row r="78" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="84"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="84"/>
-      <c r="F78" s="84"/>
-      <c r="G78" s="84"/>
-      <c r="H78" s="84"/>
-      <c r="I78" s="84"/>
-      <c r="J78" s="84"/>
-      <c r="L78" s="85"/>
-      <c r="O78" s="84"/>
+      <c r="B78" s="78"/>
+      <c r="D78" s="78"/>
+      <c r="E78" s="78"/>
+      <c r="F78" s="78"/>
+      <c r="G78" s="78"/>
+      <c r="H78" s="78"/>
+      <c r="I78" s="78"/>
+      <c r="J78" s="78"/>
+      <c r="L78" s="79"/>
+      <c r="O78" s="78"/>
       <c r="Q78" s="68"/>
       <c r="R78" s="69"/>
       <c r="S78" s="70"/>
     </row>
     <row r="79" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="84"/>
-      <c r="D79" s="84"/>
-      <c r="E79" s="84"/>
-      <c r="F79" s="84"/>
-      <c r="G79" s="84"/>
-      <c r="H79" s="84"/>
-      <c r="I79" s="84"/>
-      <c r="J79" s="84"/>
-      <c r="L79" s="85"/>
-      <c r="O79" s="84"/>
+      <c r="B79" s="78"/>
+      <c r="D79" s="78"/>
+      <c r="E79" s="78"/>
+      <c r="F79" s="78"/>
+      <c r="G79" s="78"/>
+      <c r="H79" s="78"/>
+      <c r="I79" s="78"/>
+      <c r="J79" s="78"/>
+      <c r="L79" s="79"/>
+      <c r="O79" s="78"/>
       <c r="Q79" s="68"/>
       <c r="R79" s="69"/>
       <c r="S79" s="70"/>
     </row>
     <row r="80" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="84"/>
-      <c r="D80" s="84"/>
-      <c r="E80" s="84"/>
-      <c r="F80" s="84"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="84"/>
-      <c r="I80" s="84"/>
-      <c r="J80" s="84"/>
-      <c r="L80" s="85"/>
-      <c r="O80" s="84"/>
+      <c r="B80" s="78"/>
+      <c r="D80" s="78"/>
+      <c r="E80" s="78"/>
+      <c r="F80" s="78"/>
+      <c r="G80" s="78"/>
+      <c r="H80" s="78"/>
+      <c r="I80" s="78"/>
+      <c r="J80" s="78"/>
+      <c r="L80" s="79"/>
+      <c r="O80" s="78"/>
       <c r="Q80" s="68"/>
       <c r="R80" s="69"/>
       <c r="S80" s="70"/>
     </row>
     <row r="81" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="84"/>
-      <c r="D81" s="84"/>
-      <c r="E81" s="84"/>
-      <c r="F81" s="84"/>
-      <c r="G81" s="84"/>
-      <c r="H81" s="84"/>
-      <c r="I81" s="84"/>
-      <c r="J81" s="84"/>
-      <c r="L81" s="85"/>
-      <c r="O81" s="84"/>
+      <c r="B81" s="78"/>
+      <c r="D81" s="78"/>
+      <c r="E81" s="78"/>
+      <c r="F81" s="78"/>
+      <c r="G81" s="78"/>
+      <c r="H81" s="78"/>
+      <c r="I81" s="78"/>
+      <c r="J81" s="78"/>
+      <c r="L81" s="79"/>
+      <c r="O81" s="78"/>
       <c r="Q81" s="68"/>
       <c r="R81" s="69"/>
       <c r="S81" s="70"/>
     </row>
     <row r="82" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="84"/>
-      <c r="D82" s="84"/>
-      <c r="E82" s="84"/>
-      <c r="F82" s="84"/>
-      <c r="G82" s="84"/>
-      <c r="H82" s="84"/>
-      <c r="I82" s="84"/>
-      <c r="J82" s="84"/>
-      <c r="L82" s="85"/>
-      <c r="O82" s="84"/>
+      <c r="B82" s="78"/>
+      <c r="D82" s="78"/>
+      <c r="E82" s="78"/>
+      <c r="F82" s="78"/>
+      <c r="G82" s="78"/>
+      <c r="H82" s="78"/>
+      <c r="I82" s="78"/>
+      <c r="J82" s="78"/>
+      <c r="L82" s="79"/>
+      <c r="O82" s="78"/>
       <c r="Q82" s="68"/>
       <c r="R82" s="69"/>
       <c r="S82" s="70"/>
     </row>
     <row r="83" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="84"/>
-      <c r="D83" s="84"/>
-      <c r="E83" s="84"/>
-      <c r="F83" s="84"/>
-      <c r="G83" s="84"/>
-      <c r="H83" s="84"/>
-      <c r="I83" s="84"/>
-      <c r="J83" s="84"/>
-      <c r="L83" s="85"/>
-      <c r="O83" s="84"/>
+      <c r="B83" s="78"/>
+      <c r="D83" s="78"/>
+      <c r="E83" s="78"/>
+      <c r="F83" s="78"/>
+      <c r="G83" s="78"/>
+      <c r="H83" s="78"/>
+      <c r="I83" s="78"/>
+      <c r="J83" s="78"/>
+      <c r="L83" s="79"/>
+      <c r="O83" s="78"/>
       <c r="Q83" s="68"/>
       <c r="R83" s="69"/>
       <c r="S83" s="70"/>
     </row>
     <row r="84" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="84"/>
-      <c r="D84" s="84"/>
-      <c r="E84" s="84"/>
-      <c r="F84" s="84"/>
-      <c r="G84" s="84"/>
-      <c r="H84" s="84"/>
-      <c r="I84" s="84"/>
-      <c r="J84" s="84"/>
-      <c r="L84" s="85"/>
-      <c r="O84" s="84"/>
+      <c r="B84" s="78"/>
+      <c r="D84" s="78"/>
+      <c r="E84" s="78"/>
+      <c r="F84" s="78"/>
+      <c r="G84" s="78"/>
+      <c r="H84" s="78"/>
+      <c r="I84" s="78"/>
+      <c r="J84" s="78"/>
+      <c r="L84" s="79"/>
+      <c r="O84" s="78"/>
       <c r="Q84" s="68"/>
       <c r="R84" s="69"/>
       <c r="S84" s="70"/>
     </row>
     <row r="85" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="84"/>
-      <c r="D85" s="84"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="84"/>
-      <c r="H85" s="84"/>
-      <c r="I85" s="84"/>
-      <c r="J85" s="84"/>
-      <c r="L85" s="85"/>
-      <c r="O85" s="84"/>
+      <c r="B85" s="78"/>
+      <c r="D85" s="78"/>
+      <c r="E85" s="78"/>
+      <c r="F85" s="78"/>
+      <c r="G85" s="78"/>
+      <c r="H85" s="78"/>
+      <c r="I85" s="78"/>
+      <c r="J85" s="78"/>
+      <c r="L85" s="79"/>
+      <c r="O85" s="78"/>
       <c r="Q85" s="68"/>
       <c r="R85" s="69"/>
       <c r="S85" s="70"/>
     </row>
     <row r="86" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="84"/>
-      <c r="D86" s="84"/>
-      <c r="E86" s="84"/>
-      <c r="F86" s="84"/>
-      <c r="G86" s="84"/>
-      <c r="H86" s="84"/>
-      <c r="I86" s="84"/>
-      <c r="J86" s="84"/>
-      <c r="L86" s="85"/>
-      <c r="O86" s="84"/>
+      <c r="B86" s="78"/>
+      <c r="D86" s="78"/>
+      <c r="E86" s="78"/>
+      <c r="F86" s="78"/>
+      <c r="G86" s="78"/>
+      <c r="H86" s="78"/>
+      <c r="I86" s="78"/>
+      <c r="J86" s="78"/>
+      <c r="L86" s="79"/>
+      <c r="O86" s="78"/>
       <c r="Q86" s="68"/>
       <c r="R86" s="69"/>
       <c r="S86" s="70"/>
     </row>
     <row r="87" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="84"/>
-      <c r="D87" s="84"/>
-      <c r="E87" s="84"/>
-      <c r="F87" s="84"/>
-      <c r="G87" s="84"/>
-      <c r="H87" s="84"/>
-      <c r="I87" s="84"/>
-      <c r="J87" s="84"/>
-      <c r="L87" s="85"/>
-      <c r="O87" s="84"/>
+      <c r="B87" s="78"/>
+      <c r="D87" s="78"/>
+      <c r="E87" s="78"/>
+      <c r="F87" s="78"/>
+      <c r="G87" s="78"/>
+      <c r="H87" s="78"/>
+      <c r="I87" s="78"/>
+      <c r="J87" s="78"/>
+      <c r="L87" s="79"/>
+      <c r="O87" s="78"/>
       <c r="Q87" s="68"/>
       <c r="R87" s="69"/>
       <c r="S87" s="70"/>
     </row>
     <row r="88" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="84"/>
-      <c r="D88" s="84"/>
-      <c r="E88" s="84"/>
-      <c r="F88" s="84"/>
-      <c r="G88" s="84"/>
-      <c r="H88" s="84"/>
-      <c r="I88" s="84"/>
-      <c r="J88" s="84"/>
-      <c r="L88" s="85"/>
-      <c r="O88" s="84"/>
-      <c r="Q88" s="84"/>
-      <c r="R88" s="86"/>
+      <c r="B88" s="78"/>
+      <c r="D88" s="78"/>
+      <c r="E88" s="78"/>
+      <c r="F88" s="78"/>
+      <c r="G88" s="78"/>
+      <c r="H88" s="78"/>
+      <c r="I88" s="78"/>
+      <c r="J88" s="78"/>
+      <c r="L88" s="79"/>
+      <c r="O88" s="78"/>
+      <c r="Q88" s="78"/>
+      <c r="R88" s="80"/>
     </row>
     <row r="89" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="84"/>
-      <c r="D89" s="84"/>
-      <c r="E89" s="84"/>
-      <c r="F89" s="84"/>
-      <c r="G89" s="84"/>
-      <c r="H89" s="84"/>
-      <c r="I89" s="84"/>
-      <c r="J89" s="84"/>
-      <c r="L89" s="85"/>
-      <c r="O89" s="84"/>
-      <c r="Q89" s="84"/>
-      <c r="R89" s="86"/>
+      <c r="B89" s="78"/>
+      <c r="D89" s="78"/>
+      <c r="E89" s="78"/>
+      <c r="F89" s="78"/>
+      <c r="G89" s="78"/>
+      <c r="H89" s="78"/>
+      <c r="I89" s="78"/>
+      <c r="J89" s="78"/>
+      <c r="L89" s="79"/>
+      <c r="O89" s="78"/>
+      <c r="Q89" s="78"/>
+      <c r="R89" s="80"/>
     </row>
     <row r="90" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="84"/>
-      <c r="D90" s="84"/>
-      <c r="E90" s="84"/>
-      <c r="F90" s="84"/>
-      <c r="G90" s="84"/>
-      <c r="H90" s="84"/>
-      <c r="I90" s="84"/>
-      <c r="J90" s="84"/>
-      <c r="L90" s="85"/>
-      <c r="O90" s="84"/>
-      <c r="Q90" s="84"/>
-      <c r="R90" s="86"/>
+      <c r="B90" s="78"/>
+      <c r="D90" s="78"/>
+      <c r="E90" s="78"/>
+      <c r="F90" s="78"/>
+      <c r="G90" s="78"/>
+      <c r="H90" s="78"/>
+      <c r="I90" s="78"/>
+      <c r="J90" s="78"/>
+      <c r="L90" s="79"/>
+      <c r="O90" s="78"/>
+      <c r="Q90" s="78"/>
+      <c r="R90" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4009,6 +4039,927 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9C612E-A53A-8C40-8DDB-4609041A44FD}">
+  <dimension ref="B1:S1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="6.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="4" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="21" customWidth="1"/>
+    <col min="15" max="15" width="72.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="115" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="116"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="20"/>
+    </row>
+    <row r="2" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="118"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="20"/>
+    </row>
+    <row r="3" spans="2:19" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="113">
+        <v>44146</v>
+      </c>
+      <c r="C3" s="114"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3">
+        <v>405</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="20"/>
+    </row>
+    <row r="5" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="2:19" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="120">
+        <v>7</v>
+      </c>
+      <c r="C7" s="122" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="120">
+        <v>1</v>
+      </c>
+      <c r="E7" s="120">
+        <f>D7*$E$4</f>
+        <v>405</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="9">
+        <v>387007502</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="120">
+        <v>8</v>
+      </c>
+      <c r="C8" s="122" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="120">
+        <v>1</v>
+      </c>
+      <c r="E8" s="120">
+        <f>D8*$E$4</f>
+        <v>405</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="9">
+        <v>532610871</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="2:19" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="120">
+        <v>15</v>
+      </c>
+      <c r="C9" s="123" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="120">
+        <v>17</v>
+      </c>
+      <c r="E9" s="120">
+        <f>D9*$E$4</f>
+        <v>6885</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="M9" s="25"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="74" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="120">
+        <v>23</v>
+      </c>
+      <c r="C10" s="122" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="120">
+        <v>1</v>
+      </c>
+      <c r="E10" s="120">
+        <f>D10*$E$4</f>
+        <v>405</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f>MID($L10,1,2)</f>
+        <v>F2</v>
+      </c>
+      <c r="N10" s="24">
+        <f>VALUE(RIGHT($L10,2))*$D10</f>
+        <v>20</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="121">
+        <v>24</v>
+      </c>
+      <c r="C11" s="123" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="121">
+        <v>2</v>
+      </c>
+      <c r="E11" s="120">
+        <f>D11*$E$4</f>
+        <v>810</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="98" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="25" t="str">
+        <f>MID($L11,1,2)</f>
+        <v>F1</v>
+      </c>
+      <c r="N11" s="99">
+        <f>VALUE(RIGHT($L11,2))*$D11</f>
+        <v>30</v>
+      </c>
+      <c r="O11" s="74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B12" s="120">
+        <v>25</v>
+      </c>
+      <c r="C12" s="122" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="120">
+        <v>2</v>
+      </c>
+      <c r="E12" s="120">
+        <f>D12*$E$4</f>
+        <v>810</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12" s="7" t="str">
+        <f>MID($L12,1,2)</f>
+        <v>F2</v>
+      </c>
+      <c r="N12" s="24">
+        <f>VALUE(RIGHT($L12,2))*$D12</f>
+        <v>50</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="124">
+        <v>91</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="25">
+        <v>2</v>
+      </c>
+      <c r="E13" s="120">
+        <f>D13*$E$4</f>
+        <v>810</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="98" t="s">
+        <v>191</v>
+      </c>
+      <c r="M13" s="25"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="74" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B14" s="124">
+        <v>92</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1</v>
+      </c>
+      <c r="E14" s="120">
+        <f>D14*$E$4</f>
+        <v>405</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" s="74" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="124">
+        <v>93</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="25">
+        <v>4</v>
+      </c>
+      <c r="E15" s="120">
+        <f>D15*$E$4</f>
+        <v>1620</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="74" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="M15" s="25"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M18" s="68"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="70"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M19" s="68"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="70"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M20" s="68"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="70"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M21" s="68"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="70"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M22" s="68"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="70"/>
+    </row>
+    <row r="23" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="78"/>
+      <c r="H23" s="79"/>
+      <c r="K23" s="78"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="69"/>
+      <c r="O23" s="70"/>
+    </row>
+    <row r="24" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="H24" s="79"/>
+      <c r="K24" s="78"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="70"/>
+    </row>
+    <row r="25" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="H25" s="79"/>
+      <c r="K25" s="78"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="70"/>
+    </row>
+    <row r="26" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="H26" s="79"/>
+      <c r="K26" s="78"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="69"/>
+      <c r="O26" s="81"/>
+    </row>
+    <row r="27" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="H27" s="79"/>
+      <c r="K27" s="78"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="81"/>
+    </row>
+    <row r="28" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="H28" s="79"/>
+      <c r="K28" s="78"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="70"/>
+    </row>
+    <row r="29" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="K29" s="78"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="70"/>
+    </row>
+    <row r="30" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="H30" s="79"/>
+      <c r="K30" s="78"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="70"/>
+    </row>
+    <row r="31" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="H31" s="79"/>
+      <c r="K31" s="78"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="70"/>
+    </row>
+    <row r="32" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="H32" s="79"/>
+      <c r="K32" s="78"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="70"/>
+    </row>
+    <row r="33" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="H33" s="79"/>
+      <c r="K33" s="78"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="70"/>
+    </row>
+    <row r="34" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="H34" s="79"/>
+      <c r="K34" s="78"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="70"/>
+    </row>
+    <row r="35" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="H35" s="79"/>
+      <c r="K35" s="78"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="70"/>
+    </row>
+    <row r="36" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="H36" s="79"/>
+      <c r="K36" s="78"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="70"/>
+    </row>
+    <row r="37" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="H37" s="79"/>
+      <c r="K37" s="78"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="70"/>
+    </row>
+    <row r="38" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="H38" s="79"/>
+      <c r="K38" s="78"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="70"/>
+    </row>
+    <row r="39" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="H39" s="79"/>
+      <c r="K39" s="78"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="70"/>
+    </row>
+    <row r="40" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="78"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="H40" s="79"/>
+      <c r="K40" s="78"/>
+      <c r="M40" s="68"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="70"/>
+    </row>
+    <row r="41" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="78"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="78"/>
+      <c r="F41" s="78"/>
+      <c r="H41" s="79"/>
+      <c r="K41" s="78"/>
+      <c r="M41" s="68"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="70"/>
+    </row>
+    <row r="42" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="H42" s="79"/>
+      <c r="K42" s="78"/>
+      <c r="M42" s="68"/>
+      <c r="N42" s="69"/>
+      <c r="O42" s="70"/>
+    </row>
+    <row r="43" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="78"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="78"/>
+      <c r="H43" s="79"/>
+      <c r="K43" s="78"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="70"/>
+    </row>
+    <row r="44" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="78"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="78"/>
+      <c r="H44" s="79"/>
+      <c r="K44" s="78"/>
+      <c r="M44" s="68"/>
+      <c r="N44" s="69"/>
+      <c r="O44" s="70"/>
+    </row>
+    <row r="45" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="H45" s="79"/>
+      <c r="K45" s="78"/>
+      <c r="M45" s="68"/>
+      <c r="N45" s="69"/>
+      <c r="O45" s="70"/>
+    </row>
+    <row r="46" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="78"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+      <c r="H46" s="79"/>
+      <c r="K46" s="78"/>
+      <c r="M46" s="68"/>
+      <c r="N46" s="69"/>
+      <c r="O46" s="70"/>
+    </row>
+    <row r="47" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="78"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="78"/>
+      <c r="H47" s="79"/>
+      <c r="K47" s="78"/>
+      <c r="M47" s="68"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="70"/>
+    </row>
+    <row r="48" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="78"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="78"/>
+      <c r="F48" s="78"/>
+      <c r="H48" s="79"/>
+      <c r="K48" s="78"/>
+      <c r="M48" s="68"/>
+      <c r="N48" s="69"/>
+      <c r="O48" s="70"/>
+    </row>
+    <row r="49" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="78"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="H49" s="79"/>
+      <c r="K49" s="78"/>
+      <c r="M49" s="68"/>
+      <c r="N49" s="69"/>
+      <c r="O49" s="70"/>
+    </row>
+    <row r="50" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="78"/>
+      <c r="D50" s="78"/>
+      <c r="E50" s="78"/>
+      <c r="F50" s="78"/>
+      <c r="H50" s="79"/>
+      <c r="K50" s="78"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="69"/>
+      <c r="O50" s="70"/>
+    </row>
+    <row r="51" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="78"/>
+      <c r="D51" s="78"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="H51" s="79"/>
+      <c r="K51" s="78"/>
+      <c r="M51" s="68"/>
+      <c r="N51" s="69"/>
+      <c r="O51" s="70"/>
+    </row>
+    <row r="52" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="78"/>
+      <c r="D52" s="78"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
+      <c r="H52" s="79"/>
+      <c r="K52" s="78"/>
+      <c r="M52" s="68"/>
+      <c r="N52" s="69"/>
+      <c r="O52" s="70"/>
+    </row>
+    <row r="53" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="78"/>
+      <c r="D53" s="78"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="78"/>
+      <c r="H53" s="79"/>
+      <c r="K53" s="78"/>
+      <c r="M53" s="68"/>
+      <c r="N53" s="69"/>
+      <c r="O53" s="70"/>
+    </row>
+    <row r="54" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="78"/>
+      <c r="D54" s="78"/>
+      <c r="E54" s="78"/>
+      <c r="F54" s="78"/>
+      <c r="H54" s="79"/>
+      <c r="K54" s="78"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="69"/>
+      <c r="O54" s="70"/>
+    </row>
+    <row r="55" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="78"/>
+      <c r="D55" s="78"/>
+      <c r="E55" s="78"/>
+      <c r="F55" s="78"/>
+      <c r="H55" s="79"/>
+      <c r="K55" s="78"/>
+      <c r="M55" s="68"/>
+      <c r="N55" s="69"/>
+      <c r="O55" s="70"/>
+    </row>
+    <row r="56" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="78"/>
+      <c r="D56" s="78"/>
+      <c r="E56" s="78"/>
+      <c r="F56" s="78"/>
+      <c r="H56" s="79"/>
+      <c r="K56" s="78"/>
+      <c r="M56" s="78"/>
+      <c r="N56" s="80"/>
+    </row>
+    <row r="57" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="78"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="78"/>
+      <c r="F57" s="78"/>
+      <c r="H57" s="79"/>
+      <c r="K57" s="78"/>
+      <c r="M57" s="78"/>
+      <c r="N57" s="80"/>
+    </row>
+    <row r="58" spans="2:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="78"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="78"/>
+      <c r="F58" s="78"/>
+      <c r="H58" s="79"/>
+      <c r="K58" s="78"/>
+      <c r="M58" s="78"/>
+      <c r="N58" s="80"/>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E1048576" s="120"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EAADE6-4264-DE47-A067-ABBE604B6FE0}">
   <dimension ref="A1:Y83"/>
   <sheetViews>
@@ -4037,10 +4988,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="81"/>
+      <c r="C1" s="116"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -4056,10 +5007,10 @@
       <c r="T1" s="20"/>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="118"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -4075,10 +5026,10 @@
       <c r="T2" s="20"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78">
+      <c r="B3" s="113">
         <v>44146</v>
       </c>
-      <c r="C3" s="79"/>
+      <c r="C3" s="114"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>

</xml_diff>